<commit_message>
Built links and addded to Links tab of the spreadsheet for Season 16
</commit_message>
<xml_diff>
--- a/Spreadsheets/R_L_GMM_16_1.xlsx
+++ b/Spreadsheets/R_L_GMM_16_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganthomas/Development/gmm_repo/gmm-more/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3205E31-E854-F040-976A-66C051C901F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD341C2-B9DF-3748-9035-389AFBE5A3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="1276">
   <si>
     <t>YouTube Playlist Export</t>
   </si>
@@ -3852,6 +3852,18 @@
   </si>
   <si>
     <t>LTAT -- The first ep. Rhett's dad and Stevie watch embarrasing Rhett clips</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch_videos?video_ids=5KS99ERXM_4,1HEQWAkwinw,oTFnXvzXR7g,hYuWk5qCVCo,aS5dRxrO8GY,LVLaxzfnXfc,alO7IFfuBTY,Q7CefmP4hgU,eCwD5iuQdyY,eM7FWAjrzTY,jgExPhmyTJQ,geCChB4XjgM,JULKTln3SCI,BXuUJJSe4o0,s-E_8JlIxRw,HtLrfQNUXvw,hrR2CVgh0CE,GmTwuRi0BOg,3yFs3viT4JU,GeOPTYHXj2s,OU5PjPPQ8qk,VTCfwm3lsTk,sK8e-x87fvs,o6EXs20vdCc,mYF_HGcAsGc,ja7x5x9iBhE,NqBL3VA3Zc4,VeTtEtXc_60,wipvkwFPL5g,nGVuYfw5OWY,5K3GCTNfQnI,-7qivi6yBmc,4LLuE9kDd1g,N_Elz7F_ySI,qnLjBr6N2mE,_Cg5BeSfz48,oT644VQkWMs,NSbeXwFpagI,UeQR6Lo1mmg,d2e3QjAlFI4,vFzOZYwE3bo,X_cCIxiyCnY,Vod5Zd7GYCk,ny_M-MydWWs,4RqD_N5q3e4,B11tPqVaspw,UgxFTWou8TM,2vGFbrfo8zU,E9SeECaq30g,tC2JB5fOfsM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch_videos?video_ids=4NmSku4EguU,iZ8_WVGzU9c,SvzTGwmRmgg,hMlpgj8mDeQ,ROOBsMO1L_o,fvc8kRiqgus,d7E0QMCmQCU,FhSYyFKq7bE,CWjv9Y8TlKA,DhgxHtE8ISk,OeOoAH9RxOc,l95fImsjY9A,U7UWNinx7X8,_KVqZJCTsgc,wYtDNhxX4KY,39ZrDYSSfM8,OKJar2QMco0,8COfcrYVkos,6CPhdDwTViM,Go2Hp9Sk9vM,e3qMuO5sEO4,9zvFa_TN4GU,p2asguzWKVI,7QqZ6iYW3yc,03aEKimjqDo,F2Q3EAAL1F4,n9diFTyh66g,93Vnglc1d6w,TfAPuWq8P7w,DONzfJ-FEN8,LtWXwj_ZXAI,yNRMg_5uXdI,LVg81fEZAxk,79KYNmo-kYM,YhRThhv2-X8,LWdLr53VMJs,_yPlCU7S-3A,vxp3UECqK0Y,nAXtpbEzz4M,KvRzwWvnPAs,bFD7iylFwKo,d1rpCZ2dUwY,Pu_oraX4wTc,YKdLWTppfWU,cWf1iu64v80,JdImMDIEFxQ,6xKSG6bemyY,DEUQjAnIwn0,nvXiPz4y_Ts,m8euM4qdsw0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch_videos?video_ids=jNz4Bl87Xs8,wuQr6WWGeQE,p3BD-RKWn24,c3mLP9somBk,0Y9JUJmhj-o,qqw_tEAUqcY,LknSTdUpqA0,CXe8u83Sf_A,JSa5gYBEGL0,Nswtr-bG7s8,_RSojioTtUU,8yAYP7VeLB0,xhEyw-L5x44,QhBspbgNp7A,Fon7og7w4Yw,yVBcdunS7s4,rJUpsiNcki4,C9-Givrp-Lw,BfgQoeHyfms,tMFHfycSG80,QSWaPrU7NoQ,tuVT262jyug,ShSaPs0xaYE,geZjoLe-9Nw,5jCheDCLuLk,yNsXGT2JHIk,E5eEJxnPnNI,QwGTlBfNrqk,pDPsgJFNDUc,TcHA47yUnSM,SAZChYZwXEM,BLcu9k8Aun0,afTv-DVZBTo,FvGV2rs4d-w,UQYLfagetXU,A3yxyaf9obA,eYvCpsGD1XQ,X8hizejjGcE,3L_tSenrIF4,FdgxpiiSgkM,iRg_abVNUXw,g8ELDyzYl0s,PGIET2pTCa0,u1bHR3ecJTY,mUl9ezuRPKw,pmLCSnX6Mh0,XnHq9IkQ4f4,3WDr9k6RzVA,LT_e0ERaBVs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch_videos?video_ids=iQqwglUCPHo,l6fSYl2PyYo,x9QtifIu92Q,L4gPjIIlvEs,xaaHASNQlrA,1ybJqWMJdNc,T1qjjr2V-7g,-5x9cssGR1E,C9FBa70w55c,TXCdzqSrah4,PoC_7spKNok,eN-qlPP6BI8,GVn4GyTgQkA,3r_2HHbezG0,scAqxWW3934,EN1DtjV7oPo,mB31x23bB5g,TzMyhoKQ294,N1PcdFRIx3A,vJyD3uFlnNM,poA9dQcqQ5c,GrwKVXNc7_o,vcRVuAzee-A,R3bIU46HvhQ,gIHt5QpXRfs,dv7itsHcRwY,nF3RvxlBdD0</t>
   </si>
 </sst>
 </file>
@@ -4016,7 +4028,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4220,6 +4232,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -4408,7 +4426,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4428,12 +4446,13 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4790,40 +4809,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2F190B-AE94-A14A-AB62-01553BCC8E93}">
-  <dimension ref="A7:B17"/>
+  <dimension ref="A7:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>967</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>673</v>
       </c>
@@ -4831,36 +4850,48 @@
         <v>669</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="9" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="9" t="s">
         <v>677</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1275</v>
       </c>
     </row>
   </sheetData>
@@ -4872,8 +4903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J88" sqref="J88"/>
+    <sheetView showGridLines="0" topLeftCell="C73" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78:I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4885,22 +4916,23 @@
     <col min="5" max="5" width="43" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -4918,28 +4950,28 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>671</v>
       </c>
     </row>
@@ -8735,19 +8767,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8765,28 +8797,28 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>683</v>
       </c>
     </row>
@@ -11272,7 +11304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7D142B-1817-4B41-9B6B-B1ABD3656E7C}">
   <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
@@ -11285,19 +11317,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -11315,28 +11347,28 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>968</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>969</v>
       </c>
     </row>
@@ -13660,19 +13692,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Added show breakouts to Link tab of spreadsheet.
</commit_message>
<xml_diff>
--- a/Spreadsheets/R_L_GMM_16_1.xlsx
+++ b/Spreadsheets/R_L_GMM_16_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganthomas/Development/gmm_repo/gmm-more/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD341C2-B9DF-3748-9035-389AFBE5A3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29299457-3828-DD47-9CDA-EA4A14CD4283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="1276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="1280">
   <si>
     <t>YouTube Playlist Export</t>
   </si>
@@ -3864,6 +3864,18 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch_videos?video_ids=iQqwglUCPHo,l6fSYl2PyYo,x9QtifIu92Q,L4gPjIIlvEs,xaaHASNQlrA,1ybJqWMJdNc,T1qjjr2V-7g,-5x9cssGR1E,C9FBa70w55c,TXCdzqSrah4,PoC_7spKNok,eN-qlPP6BI8,GVn4GyTgQkA,3r_2HHbezG0,scAqxWW3934,EN1DtjV7oPo,mB31x23bB5g,TzMyhoKQ294,N1PcdFRIx3A,vJyD3uFlnNM,poA9dQcqQ5c,GrwKVXNc7_o,vcRVuAzee-A,R3bIU46HvhQ,gIHt5QpXRfs,dv7itsHcRwY,nF3RvxlBdD0</t>
+  </si>
+  <si>
+    <t>1455-1479</t>
+  </si>
+  <si>
+    <t>1480-1504</t>
+  </si>
+  <si>
+    <t>1505-1529</t>
+  </si>
+  <si>
+    <t>1530-1549</t>
   </si>
 </sst>
 </file>
@@ -4449,10 +4461,10 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4812,7 +4824,7 @@
   <dimension ref="A7:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4826,21 +4838,33 @@
       <c r="A8">
         <v>1</v>
       </c>
+      <c r="B8" t="s">
+        <v>1276</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
+      <c r="B9" t="s">
+        <v>1277</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
+      <c r="B10" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
+      <c r="B11" t="s">
+        <v>1279</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -4876,7 +4900,7 @@
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>676</v>
       </c>
       <c r="C16" t="s">
@@ -4887,7 +4911,7 @@
       <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>677</v>
       </c>
       <c r="C17" t="s">
@@ -4920,19 +4944,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8753,8 +8777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AA8892-3CBD-914A-97B0-ABA99B970016}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78:L97"/>
+    <sheetView showGridLines="0" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8767,19 +8791,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -11317,19 +11341,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -13692,19 +13716,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Built out methods on Season 15 to create links.
</commit_message>
<xml_diff>
--- a/Spreadsheets/R_L_GMM_16_1.xlsx
+++ b/Spreadsheets/R_L_GMM_16_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganthomas/Development/gmm_repo/gmm-more/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29299457-3828-DD47-9CDA-EA4A14CD4283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1136BDF3-E015-B743-A0C6-53D1CD4B9A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="3" r:id="rId1"/>
@@ -4823,7 +4823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2F190B-AE94-A14A-AB62-01553BCC8E93}">
   <dimension ref="A7:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4927,8 +4927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C73" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78:I93"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8777,8 +8777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AA8892-3CBD-914A-97B0-ABA99B970016}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B76" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8788,6 +8788,7 @@
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -8862,6 +8863,22 @@
       <c r="E3" s="3" t="s">
         <v>686</v>
       </c>
+      <c r="F3" t="str">
+        <f>RIGHT(E3,LEN(E3)-FIND("tu.be/",E3)-5)</f>
+        <v>4vYjRgoppNs Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G3" t="str">
+        <f>LEFT(F3,11)</f>
+        <v>4vYjRgoppNs</v>
+      </c>
+      <c r="H3" t="str">
+        <f>RIGHT(B3,11)</f>
+        <v>FYmHKmJzqh8</v>
+      </c>
+      <c r="I3" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,H3,G3)&amp;","</f>
+        <v>FYmHKmJzqh8,4vYjRgoppNs,</v>
+      </c>
       <c r="J3">
         <v>1455</v>
       </c>
@@ -8888,6 +8905,22 @@
       <c r="E4" s="5" t="s">
         <v>689</v>
       </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F67" si="0">RIGHT(E4,LEN(E4)-FIND("tu.be/",E4)-5)</f>
+        <v>ppRfbM-B96U Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G67" si="1">LEFT(F4,11)</f>
+        <v>ppRfbM-B96U</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H67" si="2">RIGHT(B4,11)</f>
+        <v>am4cODoqlA0</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I67" si="3">_xlfn.TEXTJOIN(",",TRUE,H4,G4)&amp;","</f>
+        <v>am4cODoqlA0,ppRfbM-B96U,</v>
+      </c>
       <c r="J4">
         <v>1456</v>
       </c>
@@ -8914,6 +8947,22 @@
       <c r="E5" s="3" t="s">
         <v>692</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>gYPie4_U5lE Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>gYPie4_U5lE</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>dYguibS1ltM</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="3"/>
+        <v>dYguibS1ltM,gYPie4_U5lE,</v>
+      </c>
       <c r="J5">
         <v>1457</v>
       </c>
@@ -8940,6 +8989,22 @@
       <c r="E6" s="5" t="s">
         <v>695</v>
       </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>lkFHmXlahws Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>lkFHmXlahws</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>2AH2sAdRdZI</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="3"/>
+        <v>2AH2sAdRdZI,lkFHmXlahws,</v>
+      </c>
       <c r="J6">
         <v>1458</v>
       </c>
@@ -8966,6 +9031,22 @@
       <c r="E7" s="3" t="s">
         <v>698</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>nO1kVZx-tWc Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>nO1kVZx-tWc</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>P6K2R1hj0Kg</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="3"/>
+        <v>P6K2R1hj0Kg,nO1kVZx-tWc,</v>
+      </c>
       <c r="J7">
         <v>1459</v>
       </c>
@@ -8992,6 +9073,22 @@
       <c r="E8" s="5" t="s">
         <v>701</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>ENd2bCtK9k0 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>ENd2bCtK9k0</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>G7Z4sTxy6uA</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="3"/>
+        <v>G7Z4sTxy6uA,ENd2bCtK9k0,</v>
+      </c>
       <c r="J8">
         <v>1460</v>
       </c>
@@ -9018,6 +9115,22 @@
       <c r="E9" s="3" t="s">
         <v>704</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>-1lvqzEULpY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>-1lvqzEULpY</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>oXMcjzkORD8</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="3"/>
+        <v>oXMcjzkORD8,-1lvqzEULpY,</v>
+      </c>
       <c r="J9">
         <v>1461</v>
       </c>
@@ -9044,6 +9157,22 @@
       <c r="E10" s="5" t="s">
         <v>707</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>KBj0ZiPi65Y Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>KBj0ZiPi65Y</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>K9AACJDCngk</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="3"/>
+        <v>K9AACJDCngk,KBj0ZiPi65Y,</v>
+      </c>
       <c r="J10">
         <v>1462</v>
       </c>
@@ -9070,6 +9199,22 @@
       <c r="E11" s="3" t="s">
         <v>710</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>ehYHZsvtVVE Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>ehYHZsvtVVE</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>TpgyjqVROOg</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="3"/>
+        <v>TpgyjqVROOg,ehYHZsvtVVE,</v>
+      </c>
       <c r="J11">
         <v>1463</v>
       </c>
@@ -9096,6 +9241,22 @@
       <c r="E12" s="5" t="s">
         <v>713</v>
       </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>BYRCJldta4c Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>BYRCJldta4c</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>hAt2M3eizvQ</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v>hAt2M3eizvQ,BYRCJldta4c,</v>
+      </c>
       <c r="J12">
         <v>1464</v>
       </c>
@@ -9122,6 +9283,22 @@
       <c r="E13" s="3" t="s">
         <v>716</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>WP3xYdIILSk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>WP3xYdIILSk</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>cVXIgiw4oVM</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
+        <v>cVXIgiw4oVM,WP3xYdIILSk,</v>
+      </c>
       <c r="J13">
         <v>1465</v>
       </c>
@@ -9148,6 +9325,22 @@
       <c r="E14" s="5" t="s">
         <v>719</v>
       </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>bDXkGuhf10A Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>bDXkGuhf10A</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>MyKzlxoMdco</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v>MyKzlxoMdco,bDXkGuhf10A,</v>
+      </c>
       <c r="J14">
         <v>1466</v>
       </c>
@@ -9174,6 +9367,22 @@
       <c r="E15" s="3" t="s">
         <v>722</v>
       </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>mPQIg2npwvo Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>mPQIg2npwvo</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>hGFBu55TVzE</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v>hGFBu55TVzE,mPQIg2npwvo,</v>
+      </c>
       <c r="J15">
         <v>1467</v>
       </c>
@@ -9200,6 +9409,22 @@
       <c r="E16" s="5" t="s">
         <v>725</v>
       </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>oYv-n433Kkg Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>oYv-n433Kkg</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>-nTlH-9zPEk</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="3"/>
+        <v>-nTlH-9zPEk,oYv-n433Kkg,</v>
+      </c>
       <c r="J16">
         <v>1468</v>
       </c>
@@ -9226,6 +9451,22 @@
       <c r="E17" s="3" t="s">
         <v>728</v>
       </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>g7QUigCN59o Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>g7QUigCN59o</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>mntweGmTvS4</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="3"/>
+        <v>mntweGmTvS4,g7QUigCN59o,</v>
+      </c>
       <c r="J17">
         <v>1469</v>
       </c>
@@ -9252,6 +9493,22 @@
       <c r="E18" s="5" t="s">
         <v>731</v>
       </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>D9KCMVS3QdI Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>D9KCMVS3QdI</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>1J3SsBngDUo</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="3"/>
+        <v>1J3SsBngDUo,D9KCMVS3QdI,</v>
+      </c>
       <c r="J18">
         <v>1470</v>
       </c>
@@ -9278,6 +9535,22 @@
       <c r="E19" s="3" t="s">
         <v>734</v>
       </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>ie3eBP347Zo Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>ie3eBP347Zo</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>gTaAF8cHHcM</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="3"/>
+        <v>gTaAF8cHHcM,ie3eBP347Zo,</v>
+      </c>
       <c r="J19">
         <v>1471</v>
       </c>
@@ -9304,6 +9577,22 @@
       <c r="E20" s="5" t="s">
         <v>737</v>
       </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>m5t4kw15dPI Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>m5t4kw15dPI</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>dKM34FmuDpQ</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="3"/>
+        <v>dKM34FmuDpQ,m5t4kw15dPI,</v>
+      </c>
       <c r="J20">
         <v>1472</v>
       </c>
@@ -9330,6 +9619,22 @@
       <c r="E21" s="3" t="s">
         <v>740</v>
       </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>4QZydxAsiT8 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>4QZydxAsiT8</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>ZCQE3069Qrc</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="3"/>
+        <v>ZCQE3069Qrc,4QZydxAsiT8,</v>
+      </c>
       <c r="J21">
         <v>1473</v>
       </c>
@@ -9356,6 +9661,22 @@
       <c r="E22" s="5" t="s">
         <v>743</v>
       </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>Th2WVDTn2LM Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>Th2WVDTn2LM</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>mmtKAPkccIA</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="3"/>
+        <v>mmtKAPkccIA,Th2WVDTn2LM,</v>
+      </c>
       <c r="J22">
         <v>1474</v>
       </c>
@@ -9382,6 +9703,22 @@
       <c r="E23" s="3" t="s">
         <v>746</v>
       </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>nSsK19Sp5uY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>nSsK19Sp5uY</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>DUVgD5Xn7JI</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="3"/>
+        <v>DUVgD5Xn7JI,nSsK19Sp5uY,</v>
+      </c>
       <c r="J23">
         <v>1475</v>
       </c>
@@ -9408,6 +9745,22 @@
       <c r="E24" s="5" t="s">
         <v>749</v>
       </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>TkJUvLSyieY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Photo Attributions: Benedict Cumberbatch (Gage Skidmore) Donnie Wahlberg (celebrityabc) Idris Elba (Harald Krichel) Martha Stewart (David Shankbone) Matthew McConaughey (David Torcivia) Nicole Kidman (Eva Rinaldi) Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>TkJUvLSyieY</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>QLi-AD_QQTA</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="3"/>
+        <v>QLi-AD_QQTA,TkJUvLSyieY,</v>
+      </c>
       <c r="J24">
         <v>1476</v>
       </c>
@@ -9434,6 +9787,22 @@
       <c r="E25" s="3" t="s">
         <v>752</v>
       </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>m56djOO-SzA Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>m56djOO-SzA</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>a9CaI84G30Y</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="3"/>
+        <v>a9CaI84G30Y,m56djOO-SzA,</v>
+      </c>
       <c r="J25">
         <v>1477</v>
       </c>
@@ -9460,6 +9829,22 @@
       <c r="E26" s="5" t="s">
         <v>755</v>
       </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>qA3AdBDfsjw Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>qA3AdBDfsjw</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>y1ZVSkHAczQ</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="3"/>
+        <v>y1ZVSkHAczQ,qA3AdBDfsjw,</v>
+      </c>
       <c r="J26">
         <v>1478</v>
       </c>
@@ -9486,6 +9871,22 @@
       <c r="E27" s="3" t="s">
         <v>758</v>
       </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>XVpu8AY5VHY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>XVpu8AY5VHY</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>_bEzTZ6pQg0</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="3"/>
+        <v>_bEzTZ6pQg0,XVpu8AY5VHY,</v>
+      </c>
       <c r="J27">
         <v>1479</v>
       </c>
@@ -9512,6 +9913,22 @@
       <c r="E28" s="5" t="s">
         <v>761</v>
       </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>qZph9Br5lQc Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>qZph9Br5lQc</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>HELJzE5H3GI</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="3"/>
+        <v>HELJzE5H3GI,qZph9Br5lQc,</v>
+      </c>
       <c r="J28">
         <v>1480</v>
       </c>
@@ -9538,6 +9955,22 @@
       <c r="E29" s="3" t="s">
         <v>764</v>
       </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>Y_d_91D34do Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>Y_d_91D34do</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>bliVF1tYf20</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="3"/>
+        <v>bliVF1tYf20,Y_d_91D34do,</v>
+      </c>
       <c r="J29">
         <v>1481</v>
       </c>
@@ -9564,6 +9997,22 @@
       <c r="E30" s="5" t="s">
         <v>767</v>
       </c>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>Xff2Uq3QjrU Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>Xff2Uq3QjrU</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>1r5S1M1NonE</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="3"/>
+        <v>1r5S1M1NonE,Xff2Uq3QjrU,</v>
+      </c>
       <c r="J30">
         <v>1482</v>
       </c>
@@ -9590,6 +10039,22 @@
       <c r="E31" s="3" t="s">
         <v>770</v>
       </c>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>Yhu_6Da-20I Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>Yhu_6Da-20I</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>Ogf6meMsdZ0</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="3"/>
+        <v>Ogf6meMsdZ0,Yhu_6Da-20I,</v>
+      </c>
       <c r="J31">
         <v>1483</v>
       </c>
@@ -9616,6 +10081,22 @@
       <c r="E32" s="5" t="s">
         <v>773</v>
       </c>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>k5Ng5kqUK3E Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>k5Ng5kqUK3E</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>jh1LzqVVyFs</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="3"/>
+        <v>jh1LzqVVyFs,k5Ng5kqUK3E,</v>
+      </c>
       <c r="J32">
         <v>1484</v>
       </c>
@@ -9642,6 +10123,22 @@
       <c r="E33" s="3" t="s">
         <v>776</v>
       </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>DmJiR3k8hMU Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>DmJiR3k8hMU</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>-BCdhMu7Uy4</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="3"/>
+        <v>-BCdhMu7Uy4,DmJiR3k8hMU,</v>
+      </c>
       <c r="J33">
         <v>1485</v>
       </c>
@@ -9668,6 +10165,22 @@
       <c r="E34" s="5" t="s">
         <v>779</v>
       </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>TIvmSpTYH0I Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>TIvmSpTYH0I</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>pmwC4YI0D2A</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="3"/>
+        <v>pmwC4YI0D2A,TIvmSpTYH0I,</v>
+      </c>
       <c r="J34">
         <v>1486</v>
       </c>
@@ -9694,6 +10207,22 @@
       <c r="E35" s="3" t="s">
         <v>782</v>
       </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>Quav0uK2J18 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>Quav0uK2J18</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>ZBDaeb-XcVc</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="3"/>
+        <v>ZBDaeb-XcVc,Quav0uK2J18,</v>
+      </c>
       <c r="J35">
         <v>1487</v>
       </c>
@@ -9720,6 +10249,22 @@
       <c r="E36" s="5" t="s">
         <v>785</v>
       </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>4Rf4md_Y10E Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>4Rf4md_Y10E</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>oKuQeW3CDGU</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="3"/>
+        <v>oKuQeW3CDGU,4Rf4md_Y10E,</v>
+      </c>
       <c r="J36">
         <v>1488</v>
       </c>
@@ -9746,6 +10291,22 @@
       <c r="E37" s="3" t="s">
         <v>788</v>
       </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>_zVzezC2qRY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>_zVzezC2qRY</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>mP28nymtNdM</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="3"/>
+        <v>mP28nymtNdM,_zVzezC2qRY,</v>
+      </c>
       <c r="J37">
         <v>1489</v>
       </c>
@@ -9772,6 +10333,22 @@
       <c r="E38" s="5" t="s">
         <v>791</v>
       </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>HQzRP_7PaoU Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>HQzRP_7PaoU</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>faHGd39BKyU</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="3"/>
+        <v>faHGd39BKyU,HQzRP_7PaoU,</v>
+      </c>
       <c r="J38">
         <v>1490</v>
       </c>
@@ -9798,6 +10375,22 @@
       <c r="E39" s="3" t="s">
         <v>794</v>
       </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>fKGS7IKPDEY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>fKGS7IKPDEY</v>
+      </c>
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>T6AeO7flGx8</v>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="3"/>
+        <v>T6AeO7flGx8,fKGS7IKPDEY,</v>
+      </c>
       <c r="J39">
         <v>1491</v>
       </c>
@@ -9824,6 +10417,22 @@
       <c r="E40" s="5" t="s">
         <v>797</v>
       </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>OP9Tuj_RG3Q Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>OP9Tuj_RG3Q</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>pm7GpKlXJSg</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="3"/>
+        <v>pm7GpKlXJSg,OP9Tuj_RG3Q,</v>
+      </c>
       <c r="J40">
         <v>1492</v>
       </c>
@@ -9850,6 +10459,22 @@
       <c r="E41" s="3" t="s">
         <v>799</v>
       </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>Qi1-3PzoVfk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>Qi1-3PzoVfk</v>
+      </c>
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>JOlSuAF5I2w</v>
+      </c>
+      <c r="I41" t="str">
+        <f t="shared" si="3"/>
+        <v>JOlSuAF5I2w,Qi1-3PzoVfk,</v>
+      </c>
       <c r="J41">
         <v>1493</v>
       </c>
@@ -9876,6 +10501,22 @@
       <c r="E42" s="5" t="s">
         <v>802</v>
       </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>uiQAQM-Gm-M Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>uiQAQM-Gm-M</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>y38PnLeyHlM</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="3"/>
+        <v>y38PnLeyHlM,uiQAQM-Gm-M,</v>
+      </c>
       <c r="J42">
         <v>1494</v>
       </c>
@@ -9902,6 +10543,22 @@
       <c r="E43" s="3" t="s">
         <v>805</v>
       </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>vFkKCQ4_VvQ Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>vFkKCQ4_VvQ</v>
+      </c>
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>RtXyrvEgxhs</v>
+      </c>
+      <c r="I43" t="str">
+        <f t="shared" si="3"/>
+        <v>RtXyrvEgxhs,vFkKCQ4_VvQ,</v>
+      </c>
       <c r="J43">
         <v>1495</v>
       </c>
@@ -9928,6 +10585,22 @@
       <c r="E44" s="5" t="s">
         <v>808</v>
       </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>LVv5MsNnArM Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>LVv5MsNnArM</v>
+      </c>
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>tcRs2GrzMDE</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="shared" si="3"/>
+        <v>tcRs2GrzMDE,LVv5MsNnArM,</v>
+      </c>
       <c r="J44">
         <v>1496</v>
       </c>
@@ -9954,6 +10627,22 @@
       <c r="E45" s="3" t="s">
         <v>811</v>
       </c>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>I0ILbe_FilY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>I0ILbe_FilY</v>
+      </c>
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>7xV4Ec1mY_Y</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="shared" si="3"/>
+        <v>7xV4Ec1mY_Y,I0ILbe_FilY,</v>
+      </c>
       <c r="J45">
         <v>1497</v>
       </c>
@@ -9980,6 +10669,22 @@
       <c r="E46" s="5" t="s">
         <v>814</v>
       </c>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>hX2H9T-78j0 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>hX2H9T-78j0</v>
+      </c>
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>fBABfWqSN2I</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="3"/>
+        <v>fBABfWqSN2I,hX2H9T-78j0,</v>
+      </c>
       <c r="J46">
         <v>1498</v>
       </c>
@@ -10006,6 +10711,22 @@
       <c r="E47" s="3" t="s">
         <v>817</v>
       </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>Aj-o4BTR0eI Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>Aj-o4BTR0eI</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>-rezB2W82XA</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="3"/>
+        <v>-rezB2W82XA,Aj-o4BTR0eI,</v>
+      </c>
       <c r="J47">
         <v>1499</v>
       </c>
@@ -10032,6 +10753,22 @@
       <c r="E48" s="5" t="s">
         <v>820</v>
       </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>b3WA0vv4Jn4 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>b3WA0vv4Jn4</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>G53Pdx2HAt4</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="3"/>
+        <v>G53Pdx2HAt4,b3WA0vv4Jn4,</v>
+      </c>
       <c r="J48">
         <v>1500</v>
       </c>
@@ -10058,6 +10795,22 @@
       <c r="E49" s="3" t="s">
         <v>823</v>
       </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>g1Pu8bk4epI Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>g1Pu8bk4epI</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>he5eLD7bP6c</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="3"/>
+        <v>he5eLD7bP6c,g1Pu8bk4epI,</v>
+      </c>
       <c r="J49">
         <v>1501</v>
       </c>
@@ -10084,6 +10837,22 @@
       <c r="E50" s="5" t="s">
         <v>826</v>
       </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>rQsCa440yOo Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>rQsCa440yOo</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>ZLscS8MpP3g</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="3"/>
+        <v>ZLscS8MpP3g,rQsCa440yOo,</v>
+      </c>
       <c r="J50">
         <v>1502</v>
       </c>
@@ -10110,6 +10879,22 @@
       <c r="E51" s="3" t="s">
         <v>829</v>
       </c>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>ENk1euJYrHo Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>ENk1euJYrHo</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>8a3roR4VrhQ</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="3"/>
+        <v>8a3roR4VrhQ,ENk1euJYrHo,</v>
+      </c>
       <c r="J51">
         <v>1503</v>
       </c>
@@ -10136,6 +10921,22 @@
       <c r="E52" s="5" t="s">
         <v>832</v>
       </c>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>-sHy9WYRbqs Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>-sHy9WYRbqs</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>5GT0h8wKpTY</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="3"/>
+        <v>5GT0h8wKpTY,-sHy9WYRbqs,</v>
+      </c>
       <c r="J52">
         <v>1504</v>
       </c>
@@ -10162,6 +10963,22 @@
       <c r="E53" s="3" t="s">
         <v>835</v>
       </c>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>yT3LKUvuMn4 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v>yT3LKUvuMn4</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>iknH5MIUyqU</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="3"/>
+        <v>iknH5MIUyqU,yT3LKUvuMn4,</v>
+      </c>
       <c r="J53">
         <v>1505</v>
       </c>
@@ -10188,6 +11005,22 @@
       <c r="E54" s="5" t="s">
         <v>838</v>
       </c>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>s51sQRrE2yg Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>s51sQRrE2yg</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>usDN3xK8bRg</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="3"/>
+        <v>usDN3xK8bRg,s51sQRrE2yg,</v>
+      </c>
       <c r="J54">
         <v>1506</v>
       </c>
@@ -10214,6 +11047,22 @@
       <c r="E55" s="3" t="s">
         <v>841</v>
       </c>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>0S4vlD6MWmk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>0S4vlD6MWmk</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>BT4I-8FVAm0</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="3"/>
+        <v>BT4I-8FVAm0,0S4vlD6MWmk,</v>
+      </c>
       <c r="J55">
         <v>1507</v>
       </c>
@@ -10240,6 +11089,22 @@
       <c r="E56" s="5" t="s">
         <v>844</v>
       </c>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>5enjfV3E8Hs Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v>5enjfV3E8Hs</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="2"/>
+        <v>FiqTmmWfVdg</v>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="3"/>
+        <v>FiqTmmWfVdg,5enjfV3E8Hs,</v>
+      </c>
       <c r="J56">
         <v>1508</v>
       </c>
@@ -10266,6 +11131,22 @@
       <c r="E57" s="3" t="s">
         <v>847</v>
       </c>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>jXF1s4VMzbM Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v>jXF1s4VMzbM</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="2"/>
+        <v>WtoN09cLg2Y</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="3"/>
+        <v>WtoN09cLg2Y,jXF1s4VMzbM,</v>
+      </c>
       <c r="J57">
         <v>1509</v>
       </c>
@@ -10292,6 +11173,22 @@
       <c r="E58" s="5" t="s">
         <v>850</v>
       </c>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>WZ6mx4_boQU Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v>WZ6mx4_boQU</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="2"/>
+        <v>2SdtjAF9NVY</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="3"/>
+        <v>2SdtjAF9NVY,WZ6mx4_boQU,</v>
+      </c>
       <c r="J58">
         <v>1510</v>
       </c>
@@ -10318,6 +11215,22 @@
       <c r="E59" s="3" t="s">
         <v>853</v>
       </c>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>m1_W46oamGQ Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="1"/>
+        <v>m1_W46oamGQ</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>GyCBW5-5THw</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="3"/>
+        <v>GyCBW5-5THw,m1_W46oamGQ,</v>
+      </c>
       <c r="J59">
         <v>1511</v>
       </c>
@@ -10344,6 +11257,22 @@
       <c r="E60" s="5" t="s">
         <v>856</v>
       </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>y4eOA74XLEM Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="1"/>
+        <v>y4eOA74XLEM</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>unqZGgkHlKU</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="3"/>
+        <v>unqZGgkHlKU,y4eOA74XLEM,</v>
+      </c>
       <c r="J60">
         <v>1512</v>
       </c>
@@ -10370,6 +11299,22 @@
       <c r="E61" s="3" t="s">
         <v>859</v>
       </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>OGOrpfyBjrc Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="1"/>
+        <v>OGOrpfyBjrc</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>YVX9oGegYq0</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="3"/>
+        <v>YVX9oGegYq0,OGOrpfyBjrc,</v>
+      </c>
       <c r="J61">
         <v>1513</v>
       </c>
@@ -10396,6 +11341,22 @@
       <c r="E62" s="5" t="s">
         <v>862</v>
       </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>665d6G6cr-Q Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v>665d6G6cr-Q</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>TSouY_Y6wtw</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="3"/>
+        <v>TSouY_Y6wtw,665d6G6cr-Q,</v>
+      </c>
       <c r="J62">
         <v>1514</v>
       </c>
@@ -10422,6 +11383,22 @@
       <c r="E63" s="3" t="s">
         <v>865</v>
       </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>TUCop0uOh6Q Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v>TUCop0uOh6Q</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>zcWyp6chXdE</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="3"/>
+        <v>zcWyp6chXdE,TUCop0uOh6Q,</v>
+      </c>
       <c r="J63">
         <v>1515</v>
       </c>
@@ -10448,6 +11425,22 @@
       <c r="E64" s="5" t="s">
         <v>868</v>
       </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>Fvsk_uG9lqY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="1"/>
+        <v>Fvsk_uG9lqY</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>HBWCXvsRg_I</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="3"/>
+        <v>HBWCXvsRg_I,Fvsk_uG9lqY,</v>
+      </c>
       <c r="J64">
         <v>1516</v>
       </c>
@@ -10474,6 +11467,22 @@
       <c r="E65" s="3" t="s">
         <v>871</v>
       </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>oyugg-rOBDg Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="1"/>
+        <v>oyugg-rOBDg</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="2"/>
+        <v>tYJopzoK3oQ</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="3"/>
+        <v>tYJopzoK3oQ,oyugg-rOBDg,</v>
+      </c>
       <c r="J65">
         <v>1517</v>
       </c>
@@ -10500,6 +11509,22 @@
       <c r="E66" s="5" t="s">
         <v>874</v>
       </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>1rQZrDiF8kM Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="1"/>
+        <v>1rQZrDiF8kM</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="2"/>
+        <v>xC37h9Q-_hY</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="3"/>
+        <v>xC37h9Q-_hY,1rQZrDiF8kM,</v>
+      </c>
       <c r="J66">
         <v>1518</v>
       </c>
@@ -10526,6 +11551,22 @@
       <c r="E67" s="3" t="s">
         <v>877</v>
       </c>
+      <c r="F67" t="str">
+        <f t="shared" si="0"/>
+        <v>N7DWnnZzcio Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="1"/>
+        <v>N7DWnnZzcio</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="2"/>
+        <v>JTLQnH3bx0w</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="3"/>
+        <v>JTLQnH3bx0w,N7DWnnZzcio,</v>
+      </c>
       <c r="J67">
         <v>1519</v>
       </c>
@@ -10552,6 +11593,22 @@
       <c r="E68" s="5" t="s">
         <v>879</v>
       </c>
+      <c r="F68" t="str">
+        <f t="shared" ref="F68:F97" si="4">RIGHT(E68,LEN(E68)-FIND("tu.be/",E68)-5)</f>
+        <v>nd6oa1ssHcg Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" ref="G68:G97" si="5">LEFT(F68,11)</f>
+        <v>nd6oa1ssHcg</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" ref="H68:H97" si="6">RIGHT(B68,11)</f>
+        <v>ARdFK8ji96w</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" ref="I68:I97" si="7">_xlfn.TEXTJOIN(",",TRUE,H68,G68)&amp;","</f>
+        <v>ARdFK8ji96w,nd6oa1ssHcg,</v>
+      </c>
       <c r="J68">
         <v>1520</v>
       </c>
@@ -10578,6 +11635,22 @@
       <c r="E69" s="3" t="s">
         <v>882</v>
       </c>
+      <c r="F69" t="str">
+        <f t="shared" si="4"/>
+        <v>FsnDELvewf0 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="5"/>
+        <v>FsnDELvewf0</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="6"/>
+        <v>fZHfBo6C-18</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="7"/>
+        <v>fZHfBo6C-18,FsnDELvewf0,</v>
+      </c>
       <c r="J69">
         <v>1521</v>
       </c>
@@ -10604,6 +11677,22 @@
       <c r="E70" s="5" t="s">
         <v>885</v>
       </c>
+      <c r="F70" t="str">
+        <f t="shared" si="4"/>
+        <v>FbwrrqqmrZE Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="5"/>
+        <v>FbwrrqqmrZE</v>
+      </c>
+      <c r="H70" t="str">
+        <f t="shared" si="6"/>
+        <v>sgmwGz_aqzw</v>
+      </c>
+      <c r="I70" t="str">
+        <f t="shared" si="7"/>
+        <v>sgmwGz_aqzw,FbwrrqqmrZE,</v>
+      </c>
       <c r="J70">
         <v>1522</v>
       </c>
@@ -10630,6 +11719,22 @@
       <c r="E71" s="3" t="s">
         <v>888</v>
       </c>
+      <c r="F71" t="str">
+        <f t="shared" si="4"/>
+        <v>2x5Ei_xpu6k Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="5"/>
+        <v>2x5Ei_xpu6k</v>
+      </c>
+      <c r="H71" t="str">
+        <f t="shared" si="6"/>
+        <v>MFPjygCuYrE</v>
+      </c>
+      <c r="I71" t="str">
+        <f t="shared" si="7"/>
+        <v>MFPjygCuYrE,2x5Ei_xpu6k,</v>
+      </c>
       <c r="J71">
         <v>1523</v>
       </c>
@@ -10656,6 +11761,22 @@
       <c r="E72" s="5" t="s">
         <v>891</v>
       </c>
+      <c r="F72" t="str">
+        <f t="shared" si="4"/>
+        <v>o5CgO6_qX2A Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="5"/>
+        <v>o5CgO6_qX2A</v>
+      </c>
+      <c r="H72" t="str">
+        <f t="shared" si="6"/>
+        <v>UoUeBLp5KlI</v>
+      </c>
+      <c r="I72" t="str">
+        <f t="shared" si="7"/>
+        <v>UoUeBLp5KlI,o5CgO6_qX2A,</v>
+      </c>
       <c r="J72">
         <v>1524</v>
       </c>
@@ -10682,6 +11803,22 @@
       <c r="E73" s="3" t="s">
         <v>894</v>
       </c>
+      <c r="F73" t="str">
+        <f t="shared" si="4"/>
+        <v>GePx699Yd7A Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="5"/>
+        <v>GePx699Yd7A</v>
+      </c>
+      <c r="H73" t="str">
+        <f t="shared" si="6"/>
+        <v>9_HJFOxde0s</v>
+      </c>
+      <c r="I73" t="str">
+        <f t="shared" si="7"/>
+        <v>9_HJFOxde0s,GePx699Yd7A,</v>
+      </c>
       <c r="J73">
         <v>1525</v>
       </c>
@@ -10708,6 +11845,22 @@
       <c r="E74" s="5" t="s">
         <v>897</v>
       </c>
+      <c r="F74" t="str">
+        <f t="shared" si="4"/>
+        <v>7x6zABWGoUs Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="5"/>
+        <v>7x6zABWGoUs</v>
+      </c>
+      <c r="H74" t="str">
+        <f t="shared" si="6"/>
+        <v>SqyWLVEYDHE</v>
+      </c>
+      <c r="I74" t="str">
+        <f t="shared" si="7"/>
+        <v>SqyWLVEYDHE,7x6zABWGoUs,</v>
+      </c>
       <c r="J74">
         <v>1526</v>
       </c>
@@ -10734,6 +11887,22 @@
       <c r="E75" s="3" t="s">
         <v>900</v>
       </c>
+      <c r="F75" t="str">
+        <f t="shared" si="4"/>
+        <v>lIzuDeWcdpA Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="5"/>
+        <v>lIzuDeWcdpA</v>
+      </c>
+      <c r="H75" t="str">
+        <f t="shared" si="6"/>
+        <v>pu7nhRZhzLg</v>
+      </c>
+      <c r="I75" t="str">
+        <f t="shared" si="7"/>
+        <v>pu7nhRZhzLg,lIzuDeWcdpA,</v>
+      </c>
       <c r="J75">
         <v>1527</v>
       </c>
@@ -10760,6 +11929,22 @@
       <c r="E76" s="5" t="s">
         <v>903</v>
       </c>
+      <c r="F76" t="str">
+        <f t="shared" si="4"/>
+        <v>NeUeEcePFYQ Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="5"/>
+        <v>NeUeEcePFYQ</v>
+      </c>
+      <c r="H76" t="str">
+        <f t="shared" si="6"/>
+        <v>YX-Y44S_NVw</v>
+      </c>
+      <c r="I76" t="str">
+        <f t="shared" si="7"/>
+        <v>YX-Y44S_NVw,NeUeEcePFYQ,</v>
+      </c>
       <c r="J76">
         <v>1528</v>
       </c>
@@ -10786,6 +11971,22 @@
       <c r="E77" s="3" t="s">
         <v>906</v>
       </c>
+      <c r="F77" t="str">
+        <f t="shared" si="4"/>
+        <v>YbiNUlolWBE Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="5"/>
+        <v>YbiNUlolWBE</v>
+      </c>
+      <c r="H77" t="str">
+        <f t="shared" si="6"/>
+        <v>jknOHr7I5vo</v>
+      </c>
+      <c r="I77" t="str">
+        <f t="shared" si="7"/>
+        <v>jknOHr7I5vo,YbiNUlolWBE,</v>
+      </c>
       <c r="J77">
         <v>1529</v>
       </c>
@@ -10812,6 +12013,22 @@
       <c r="E78" s="5" t="s">
         <v>909</v>
       </c>
+      <c r="F78" t="str">
+        <f t="shared" si="4"/>
+        <v>U-r3JXg7neE Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="5"/>
+        <v>U-r3JXg7neE</v>
+      </c>
+      <c r="H78" t="str">
+        <f t="shared" si="6"/>
+        <v>4aebxUf8FCw</v>
+      </c>
+      <c r="I78" t="str">
+        <f t="shared" si="7"/>
+        <v>4aebxUf8FCw,U-r3JXg7neE,</v>
+      </c>
       <c r="J78">
         <v>1530</v>
       </c>
@@ -10838,6 +12055,22 @@
       <c r="E79" s="3" t="s">
         <v>912</v>
       </c>
+      <c r="F79" t="str">
+        <f t="shared" si="4"/>
+        <v>V_vm9lvQqEk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="5"/>
+        <v>V_vm9lvQqEk</v>
+      </c>
+      <c r="H79" t="str">
+        <f t="shared" si="6"/>
+        <v>5o6xy51BK3o</v>
+      </c>
+      <c r="I79" t="str">
+        <f t="shared" si="7"/>
+        <v>5o6xy51BK3o,V_vm9lvQqEk,</v>
+      </c>
       <c r="J79">
         <v>1531</v>
       </c>
@@ -10864,6 +12097,22 @@
       <c r="E80" s="5" t="s">
         <v>915</v>
       </c>
+      <c r="F80" t="str">
+        <f t="shared" si="4"/>
+        <v>2Q9NbuT1NdM Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="5"/>
+        <v>2Q9NbuT1NdM</v>
+      </c>
+      <c r="H80" t="str">
+        <f t="shared" si="6"/>
+        <v>6jaks_F2UFU</v>
+      </c>
+      <c r="I80" t="str">
+        <f t="shared" si="7"/>
+        <v>6jaks_F2UFU,2Q9NbuT1NdM,</v>
+      </c>
       <c r="J80">
         <v>1532</v>
       </c>
@@ -10890,6 +12139,22 @@
       <c r="E81" s="3" t="s">
         <v>918</v>
       </c>
+      <c r="F81" t="str">
+        <f t="shared" si="4"/>
+        <v>HE-kmbKV0ew Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="5"/>
+        <v>HE-kmbKV0ew</v>
+      </c>
+      <c r="H81" t="str">
+        <f t="shared" si="6"/>
+        <v>veToPnVyNaE</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" si="7"/>
+        <v>veToPnVyNaE,HE-kmbKV0ew,</v>
+      </c>
       <c r="J81">
         <v>1533</v>
       </c>
@@ -10916,6 +12181,22 @@
       <c r="E82" s="5" t="s">
         <v>921</v>
       </c>
+      <c r="F82" t="str">
+        <f t="shared" si="4"/>
+        <v>4wT9SWrhKqY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="5"/>
+        <v>4wT9SWrhKqY</v>
+      </c>
+      <c r="H82" t="str">
+        <f t="shared" si="6"/>
+        <v>NJ5uQ0F3yNg</v>
+      </c>
+      <c r="I82" t="str">
+        <f t="shared" si="7"/>
+        <v>NJ5uQ0F3yNg,4wT9SWrhKqY,</v>
+      </c>
       <c r="J82">
         <v>1534</v>
       </c>
@@ -10942,6 +12223,22 @@
       <c r="E83" s="3" t="s">
         <v>924</v>
       </c>
+      <c r="F83" t="str">
+        <f t="shared" si="4"/>
+        <v>V5-NG2zm4tw Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="5"/>
+        <v>V5-NG2zm4tw</v>
+      </c>
+      <c r="H83" t="str">
+        <f t="shared" si="6"/>
+        <v>BXhOMvlvlIQ</v>
+      </c>
+      <c r="I83" t="str">
+        <f t="shared" si="7"/>
+        <v>BXhOMvlvlIQ,V5-NG2zm4tw,</v>
+      </c>
       <c r="J83">
         <v>1535</v>
       </c>
@@ -10968,6 +12265,22 @@
       <c r="E84" s="5" t="s">
         <v>927</v>
       </c>
+      <c r="F84" t="str">
+        <f t="shared" si="4"/>
+        <v>P7BZp4Letro Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="5"/>
+        <v>P7BZp4Letro</v>
+      </c>
+      <c r="H84" t="str">
+        <f t="shared" si="6"/>
+        <v>Gjl-RU2VegY</v>
+      </c>
+      <c r="I84" t="str">
+        <f t="shared" si="7"/>
+        <v>Gjl-RU2VegY,P7BZp4Letro,</v>
+      </c>
       <c r="J84">
         <v>1536</v>
       </c>
@@ -10994,6 +12307,22 @@
       <c r="E85" s="3" t="s">
         <v>930</v>
       </c>
+      <c r="F85" t="str">
+        <f t="shared" si="4"/>
+        <v>OhI2CqfHVyk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="5"/>
+        <v>OhI2CqfHVyk</v>
+      </c>
+      <c r="H85" t="str">
+        <f t="shared" si="6"/>
+        <v>loojYJaNRck</v>
+      </c>
+      <c r="I85" t="str">
+        <f t="shared" si="7"/>
+        <v>loojYJaNRck,OhI2CqfHVyk,</v>
+      </c>
       <c r="J85">
         <v>1537</v>
       </c>
@@ -11020,6 +12349,22 @@
       <c r="E86" s="5" t="s">
         <v>933</v>
       </c>
+      <c r="F86" t="str">
+        <f t="shared" si="4"/>
+        <v>7H94DAkJeO4 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="5"/>
+        <v>7H94DAkJeO4</v>
+      </c>
+      <c r="H86" t="str">
+        <f t="shared" si="6"/>
+        <v>IaqqKiky0nI</v>
+      </c>
+      <c r="I86" t="str">
+        <f t="shared" si="7"/>
+        <v>IaqqKiky0nI,7H94DAkJeO4,</v>
+      </c>
       <c r="J86">
         <v>1538</v>
       </c>
@@ -11046,6 +12391,22 @@
       <c r="E87" s="3" t="s">
         <v>936</v>
       </c>
+      <c r="F87" t="str">
+        <f t="shared" si="4"/>
+        <v>HpACpqruAH8 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="5"/>
+        <v>HpACpqruAH8</v>
+      </c>
+      <c r="H87" t="str">
+        <f t="shared" si="6"/>
+        <v>3vIHUFi4aeU</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="7"/>
+        <v>3vIHUFi4aeU,HpACpqruAH8,</v>
+      </c>
       <c r="J87">
         <v>1539</v>
       </c>
@@ -11072,6 +12433,22 @@
       <c r="E88" s="5" t="s">
         <v>939</v>
       </c>
+      <c r="F88" t="str">
+        <f t="shared" si="4"/>
+        <v>MjKQeP06IAI Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="5"/>
+        <v>MjKQeP06IAI</v>
+      </c>
+      <c r="H88" t="str">
+        <f t="shared" si="6"/>
+        <v>uE6IRLhVUwc</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="7"/>
+        <v>uE6IRLhVUwc,MjKQeP06IAI,</v>
+      </c>
       <c r="J88">
         <v>1540</v>
       </c>
@@ -11098,6 +12475,22 @@
       <c r="E89" s="3" t="s">
         <v>942</v>
       </c>
+      <c r="F89" t="str">
+        <f t="shared" si="4"/>
+        <v>AaiLYhMCxII Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="5"/>
+        <v>AaiLYhMCxII</v>
+      </c>
+      <c r="H89" t="str">
+        <f t="shared" si="6"/>
+        <v>npC5RTV7uBw</v>
+      </c>
+      <c r="I89" t="str">
+        <f t="shared" si="7"/>
+        <v>npC5RTV7uBw,AaiLYhMCxII,</v>
+      </c>
       <c r="J89">
         <v>1541</v>
       </c>
@@ -11124,6 +12517,22 @@
       <c r="E90" s="5" t="s">
         <v>945</v>
       </c>
+      <c r="F90" t="str">
+        <f t="shared" si="4"/>
+        <v>EINEXO_bbrk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="5"/>
+        <v>EINEXO_bbrk</v>
+      </c>
+      <c r="H90" t="str">
+        <f t="shared" si="6"/>
+        <v>nsi_JrB1W5I</v>
+      </c>
+      <c r="I90" t="str">
+        <f t="shared" si="7"/>
+        <v>nsi_JrB1W5I,EINEXO_bbrk,</v>
+      </c>
       <c r="J90">
         <v>1542</v>
       </c>
@@ -11150,6 +12559,22 @@
       <c r="E91" s="3" t="s">
         <v>948</v>
       </c>
+      <c r="F91" t="str">
+        <f t="shared" si="4"/>
+        <v>F6PTLCC8NRY Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="5"/>
+        <v>F6PTLCC8NRY</v>
+      </c>
+      <c r="H91" t="str">
+        <f t="shared" si="6"/>
+        <v>dzudlPkRKRU</v>
+      </c>
+      <c r="I91" t="str">
+        <f t="shared" si="7"/>
+        <v>dzudlPkRKRU,F6PTLCC8NRY,</v>
+      </c>
       <c r="J91">
         <v>1543</v>
       </c>
@@ -11176,6 +12601,22 @@
       <c r="E92" s="5" t="s">
         <v>951</v>
       </c>
+      <c r="F92" t="str">
+        <f t="shared" si="4"/>
+        <v>n9vlP28MW60 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="5"/>
+        <v>n9vlP28MW60</v>
+      </c>
+      <c r="H92" t="str">
+        <f t="shared" si="6"/>
+        <v>6myJhqHNNss</v>
+      </c>
+      <c r="I92" t="str">
+        <f t="shared" si="7"/>
+        <v>6myJhqHNNss,n9vlP28MW60,</v>
+      </c>
       <c r="J92">
         <v>1544</v>
       </c>
@@ -11202,6 +12643,22 @@
       <c r="E93" s="3" t="s">
         <v>954</v>
       </c>
+      <c r="F93" t="str">
+        <f t="shared" si="4"/>
+        <v>XNUdtdhzO2g Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="5"/>
+        <v>XNUdtdhzO2g</v>
+      </c>
+      <c r="H93" t="str">
+        <f t="shared" si="6"/>
+        <v>7mHeY1B5Xzk</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" si="7"/>
+        <v>7mHeY1B5Xzk,XNUdtdhzO2g,</v>
+      </c>
       <c r="J93">
         <v>1545</v>
       </c>
@@ -11228,6 +12685,22 @@
       <c r="E94" s="5" t="s">
         <v>957</v>
       </c>
+      <c r="F94" t="str">
+        <f t="shared" si="4"/>
+        <v>i4GAYzc0nm0 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="5"/>
+        <v>i4GAYzc0nm0</v>
+      </c>
+      <c r="H94" t="str">
+        <f t="shared" si="6"/>
+        <v>uKDAJtGfqbc</v>
+      </c>
+      <c r="I94" t="str">
+        <f t="shared" si="7"/>
+        <v>uKDAJtGfqbc,i4GAYzc0nm0,</v>
+      </c>
       <c r="J94">
         <v>1546</v>
       </c>
@@ -11254,6 +12727,22 @@
       <c r="E95" s="3" t="s">
         <v>960</v>
       </c>
+      <c r="F95" t="str">
+        <f t="shared" si="4"/>
+        <v>9rmvX8jgocw Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="5"/>
+        <v>9rmvX8jgocw</v>
+      </c>
+      <c r="H95" t="str">
+        <f t="shared" si="6"/>
+        <v>9xfNyijHoOU</v>
+      </c>
+      <c r="I95" t="str">
+        <f t="shared" si="7"/>
+        <v>9xfNyijHoOU,9rmvX8jgocw,</v>
+      </c>
       <c r="J95">
         <v>1547</v>
       </c>
@@ -11280,6 +12769,22 @@
       <c r="E96" s="5" t="s">
         <v>963</v>
       </c>
+      <c r="F96" t="str">
+        <f t="shared" si="4"/>
+        <v>TUBWf9SgyD0 Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="5"/>
+        <v>TUBWf9SgyD0</v>
+      </c>
+      <c r="H96" t="str">
+        <f t="shared" si="6"/>
+        <v>9iMdlNCprZQ</v>
+      </c>
+      <c r="I96" t="str">
+        <f t="shared" si="7"/>
+        <v>9iMdlNCprZQ,TUBWf9SgyD0,</v>
+      </c>
       <c r="J96">
         <v>1548</v>
       </c>
@@ -11305,6 +12810,22 @@
       </c>
       <c r="E97" s="3" t="s">
         <v>966</v>
+      </c>
+      <c r="F97" t="str">
+        <f t="shared" si="4"/>
+        <v>2N97uKZDToE Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="5"/>
+        <v>2N97uKZDToE</v>
+      </c>
+      <c r="H97" t="str">
+        <f t="shared" si="6"/>
+        <v>G3DsWnEDqbc</v>
+      </c>
+      <c r="I97" t="str">
+        <f t="shared" si="7"/>
+        <v>G3DsWnEDqbc,2N97uKZDToE,</v>
       </c>
       <c r="J97">
         <v>1549</v>

</xml_diff>

<commit_message>
Added Summer 2019 playlist, it includes many videos it should not.
</commit_message>
<xml_diff>
--- a/Spreadsheets/R_L_GMM_16_1.xlsx
+++ b/Spreadsheets/R_L_GMM_16_1.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganthomas/Development/gmm_repo/gmm-more/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1136BDF3-E015-B743-A0C6-53D1CD4B9A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF92C9ED-937F-EF4A-9821-898802B52F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Links" sheetId="3" r:id="rId1"/>
     <sheet name="Season16" sheetId="1" r:id="rId2"/>
-    <sheet name="Season15" sheetId="4" r:id="rId3"/>
-    <sheet name="Season14" sheetId="5" r:id="rId4"/>
-    <sheet name="Season1" sheetId="2" r:id="rId5"/>
+    <sheet name="Summer2019playlist" sheetId="6" r:id="rId3"/>
+    <sheet name="Season15" sheetId="4" r:id="rId4"/>
+    <sheet name="Season14" sheetId="5" r:id="rId5"/>
+    <sheet name="Season1" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="1280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="1479">
   <si>
     <t>YouTube Playlist Export</t>
   </si>
@@ -3876,6 +3877,603 @@
   </si>
   <si>
     <t>1530-1549</t>
+  </si>
+  <si>
+    <t>Can we guess where in the world these Dunkin Donuts options hail from? GMM #1339 Watch today's GMMore: https://youtu.be/s-ix92hVKMQ Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>International Dunkin Donuts Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XQSvN2Wd5MQ</t>
+  </si>
+  <si>
+    <t>LaurDIY &amp; Alex Wassabi try to guess what we deep fried in this game of freaky fried mystery foods. GMM #1335 Thanks to Lauren &amp; Alex for hosting this episode of Good Mythical Summer! Check them out here: LaurDIY: https://www.youtube.com/LaurDIY Alex Wassabi: https://www.youtube.com/wassabi Watch today's GMMore: https://youtu.be/KLSkvMzj0Ak Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What Did We Deep Fry? ft. LaurDIY &amp; Alex Wassabi (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9aPS1OHwp1g</t>
+  </si>
+  <si>
+    <t>We're tasting popular vanilla ice creams to decide which grocery store brand truly makes us scream for ice cream. GMM #1336 Watch today's GMMore: https://youtu.be/o0P78KNN01M Want more GMS? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Blind Ice Cream Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MidgYgFwgTI</t>
+  </si>
+  <si>
+    <t>Which hot dog is the top dog? Today we're tasting America's favorite hot dog styles to decide which is truly the top hot dog. GMM #1348 Watch today's GMMore: https://youtu.be/976cBg_gwYM Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What's The Best Hot Dog Style? Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nIf2V0OH6KY</t>
+  </si>
+  <si>
+    <t>Can we guess what celebrities ate to bulk up or slim down for their most physically extreme movie roles? GMM #1334 Watch today's GMMore: https://youtu.be/UXnc_HBjzPo Want more GMS? Watch from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Extreme Celebrity Diet Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0j1YJ78oSaU</t>
+  </si>
+  <si>
+    <t>A taste for human toes? How about their mom's feces? Can Link guess which of these cute animals are actually evil beasts? GMM #1337 Watch today's GMMore: https://youtu.be/QwNf7mWQmFM Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>7 Cute But Evil Animals</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z0ekMVs1V1E</t>
+  </si>
+  <si>
+    <t>Tide Pods? Fish Guts? Today we ask the age old question - will it slip-n-slide? GMM #1333 Get our limited edition Summer Camp tee at http://mythical.store Watch today's GMMore: https://youtu.be/-humHGoKXzw Want more GMS? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Will It Slip-N-Slide? (EXPERIMENT)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ys6KVWA4okw</t>
+  </si>
+  <si>
+    <t>We guess which perfume is being sold in these absolutely absurd perfume commercials? GMM #1343 Watch today's GMMore: https://youtu.be/FNlwbta04Po Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>World's Most Ridiculous Perfume Commercials (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PHop7hery_U</t>
+  </si>
+  <si>
+    <t>Nick Offerman &amp; Kiersey Clemons turn cringey dad texts into smooth rocking classic dad songs GMM #1338 Thanks to Nick and Kiersey for hosting this episode of Good Mythical Summer! Check out their movie "Hearts Beat Loud" in theaters now. Watch the trailer here: https://www.youtube.com/watch?v=PXNOg_SK7Vs Watch today's GMMore: https://youtu.be/1yAJ4MH8mss Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Nick Offerman Sings Dad Songs w/ Kiersey Clemons</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NaaFLyxlyG0</t>
+  </si>
+  <si>
+    <t>Can we guess what weird non-water things we're swimming in today? GMM #1342 Watch today's GMMore: https://youtu.be/O5Xia4_tqzY Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What Are We Swimming In? (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AZpo33GgH4k</t>
+  </si>
+  <si>
+    <t>Safiya Nygaard &amp; Tyler Williams are filling their mouths and trying to guess what's in their mouths. GMM #1341 Thanks to Safiya &amp; Tyler for hosting GMS! Check them out at: Safiya's Channel: https://www.youtube.com/safiyanygaard Tyler's Channel: https://www.youtube.com/channel/UCc6BTuuTzfMLKj_RgwuDnQw Watch today's GMMore: https://youtu.be/OXGDwVKHAEU Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What's In My Mouth? w/ Safiya Nygaard &amp; Tyler Williams</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LWEGoDJK-cU</t>
+  </si>
+  <si>
+    <t>Can we guess who pukes and who keeps their cookies down in these roller coaster videos? GMM #1340 Watch today's GMMore: https://youtu.be/679xaKECVHo Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Will They Puke?: Roller Coaster Edition</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wScW1v10MBE</t>
+  </si>
+  <si>
+    <t>Food commercials look amazing...but does the TV-ready styled food actually taste amazing? GMM #1345 Watch today's GMMore: https://youtu.be/Uzq7F3ImZRA Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Commercial Styled Food Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Mq3la1i1gzM</t>
+  </si>
+  <si>
+    <t>Will De'arra or Ken chicken out first in this NASTY GAME of truth or dare? GMM #1353 Thanks to De'arra &amp; Ken for hosting today's episode! Check them out: De'arra &amp; Ken 4 Life: https://goo.gl/Wsta5j DK4L Vlogs: https://goo.gl/G8V9LR Watch today's GMMore: https://youtu.be/ELBP8yU-RI4 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Relationship Chicken ft. De'arra &amp; Ken 4 Life (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2FHf2baospw</t>
+  </si>
+  <si>
+    <t>Do Jon &amp; Noah know their iconic Disney movie foods or are they more into the Minions than Mickey Mouse? GMM #1344 Thanks to Jon &amp; Noah for hosting today's GMS, check them out at: Noah Cyrus: https://www.instagram.com/noahcyrus/ https://twitter.com/noahcyrus/ https://facebook.com/noahcyrus/ Jon Cozart: https://www.youtube.com/user/Paint Watch today's GMMore: https://youtu.be/mLvbZAdGsZY Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Check our Noah's latest single, Team, here: Spotify: http://smarturl.it/AlwaysBeOnYourTeam/spotify Apple Music: http://smarturl.it/AlwaysBeOnYourTeam/applemusic iTunes: http://smarturl.it/AlwaysBeOnYourTeam/itunes Amazon: http://smarturl.it/AlwaysBeOnYourTeam/az Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Disney Movie Food Challenge w/ Jon Cozart &amp; Noah Cyrus</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MVpHIU2pqEM</t>
+  </si>
+  <si>
+    <t>The Try Guys try their hand at cornhole to avoid having to chow down on nasty corn dogs. GMM #1347 Thanks to the Try Guys for hosting GMM today! Check out their new channel today: https://goo.gl/pdUjr4 Watch today's GMMore: https://youtu.be/9Nn4F5F6klg Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Nasty Corn Dog Taste Test ft. Try Guys (Cornhole Game)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=W1_87l1k9Bw</t>
+  </si>
+  <si>
+    <t>How well does Hot Ones host, Sean Evans, know his habanero flavored snack foods? We put him &amp; Alex to the test! GMM #1350 Thanks to Sean Evans for hosting GMS today! Check him out at: Hot Ones: https://goo.gl/xjU8rR Twitter: https://twitter.com/seanseaevans Watch today's GMMore: https://youtu.be/a74US2GPxs4 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Habanero Snack Taste Test ft. Sean Evans</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=s20jPiasLDg</t>
+  </si>
+  <si>
+    <t>Why'd Nicki Minaj end up behind bars? We test our celebrity arrest knowledge in today's criminally hard game! GMM #1349 Watch today's GMMore: https://youtu.be/1EvYN7E18AI Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What Was The Celebrity Arrested For? (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gti0BTWCrfA</t>
+  </si>
+  <si>
+    <t>It's hard to keep your cool at VidCon...especially in horse manure! This episode contains an advertisement from Hasbro. Grab your own 'Don't Lose Your Cool' game here: https://go.hasb.ro/2IvTk70 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Taking A Bath In Horse Manure (Don’t Lose Your Cool)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6KENbOG4hvI</t>
+  </si>
+  <si>
+    <t>Rhett and Link test 5 ways to beat the heat this summer -- including legs covered in bird poo. GMM #1351 Watch today's GMMore: https://youtu.be/x81k9pKkkWQ Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>We Test 5 Ways To Beat the Heat</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=03q3UG_3TrM</t>
+  </si>
+  <si>
+    <t>Do we still recognize our favorite TV shows after they're been remade in foreign countries? GMM #1346 Watch today's GMMore: https://youtu.be/hcJIGQzH4SQ Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>7 Foreign Remakes of American TV Shows (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-1DHvamxCxU</t>
+  </si>
+  <si>
+    <t>They might WWE Superstars but are The Miz &amp; Maryse also baby food taste testing champions? We put them to the test! GMM#1356 Thanks to The Miz &amp; Maryse for hosting GMM! Don't miss the premiere of 'Miz &amp; Mrs' on USA: https://goo.gl/WxRnBG The Miz: https://twitter.com/mikethemiz Maryse: https://twitter.com/marysemizanin Watch today's GMMore: https://youtu.be/sllYuOndRyg Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Mystery Baby Food Taste Test ft The Miz &amp; Maryse</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nghhhCJOIEg</t>
+  </si>
+  <si>
+    <t>Can we believe it's now butter? Or are these new butter options better off unchurned? GMM #1354 Watch today's GMMore: https://youtu.be/nZ0n5PelEqc Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Will It Butter? Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HJ1-Wjk7mj4</t>
+  </si>
+  <si>
+    <t>Threadbanger's Corinne &amp; Rob give some popular watermelon hacks mythical make overs -- including liquid nitrogen melon ice pops. GMM #1359 Thanks to Threadbanger for hosting GMM today! Check them out: https://www.youtube.com/ThreadBanger https://twitter.com/Threadbanger Watch today's GMMore: https://youtu.be/x2rcnIHjTTA Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Liquid Nitrogen Watermelon Taste Test ft. ThreadBanger</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ia1K304HuhM</t>
+  </si>
+  <si>
+    <t>Can Link guess how much people are willing to spend on these outrageously expensive meals? GMM #1352 Watch today's GMMore: https://youtu.be/2gVLBIwYXfY Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>7 Most Expensive Meals In The World</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4febC1iYbZ8</t>
+  </si>
+  <si>
+    <t>Have you ever snacked down on one of these taste-a-like knock off food brands? GMM #1355 Watch today's GMMore: https://youtu.be/nMpGrm_2BQM Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Unbelievable Knock Off Brands (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ilriGIFE0EA</t>
+  </si>
+  <si>
+    <t>Are these discontinued snacks good enough to bring back? Or should we leave these 50 year old pretzels on the shelf? GMM #1358 Watch today's GMMore: https://youtu.be/qHTPTwiElU4 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>50 Year Old Pretzel Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5rIzlDYTARE</t>
+  </si>
+  <si>
+    <t>Will Stevie's Uterus Chili Cheese Fries be love at first taste test? FF#003 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical: Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Uterus Chili Cheese Fries Taste Test | FOOD FEARS</t>
+  </si>
+  <si>
+    <t>Mythical Kitchen</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=i884G4L_s7o</t>
+  </si>
+  <si>
+    <t>Will Jordan have a new taste for testicles after he tries Josh’s bull testicle breakfast burrito? FF #005 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Bull Testicle Breakfast Burrito Taste Test | FOOD FEARS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CrBdHKsyDwQ</t>
+  </si>
+  <si>
+    <t>Josh works his magic in the kitchen to create Taco Bell’s next viral menu item, the 9-Layer CrunchWrapiChanga, in the very first Future Fast Food episode! FFF #001 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Tweet @TacoBell using #FutureFastFood so everyone can taste this! https://twitter.com/tacobell?s=09 Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Taco Bell Deep Fried Crunchwrap Taste Test | FUTURE FAST FOOD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=38DRQWl8n6Q</t>
+  </si>
+  <si>
+    <t>Josh takes on the Golden Arches and creates McDonald's next big menu item - the Kimchi Bacon Ramen Big Mac! FFF #002 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Tweet @McDonalds using #FutureFastFood so everyone can taste this! https://twitter.com/McDonalds Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>McDonald's Kimchi Bacon Ramen Big Mac Taste Test | FUTURE FAST FOOD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XvT5YT5tFFE</t>
+  </si>
+  <si>
+    <t>Josh anticipates Pizza Hut’s next big move with the most Instagrammable dish - the Four Way Pizza! FFF #003 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Tell Pizza Hut that you're ready for the Four Way! https://ctt.ac/be697 Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Pizza Hut Four Way Pizza Taste Test | FUTURE FAST FOOD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sr7__XCxXcs</t>
+  </si>
+  <si>
+    <t>Our very own chef Josh whips up a savory Lobster Champagne Brunch Burger he predicts to hit every Carl's Jr. restaurant! FFF #005 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Tweet @CarlsJr using #FutureFastFood so everyone can taste this! https://ctt.ac/y4iSg Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Carl’s Jr. Lobster Champagne Brunch Burger Taste Test | FUTURE FAST FOOD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=uqjVswzvYYo</t>
+  </si>
+  <si>
+    <t>We're crowning the Chicken Wing King today in a taste showdown of restaurant chicken wing offerings. Enjoy this blind chicken wing taste test! GMM #1357 Watch today's GMMore: https://youtu.be/NaQViFWuO9g Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Who Makes The Best Chicken Wings? Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MBPdKxlazD0</t>
+  </si>
+  <si>
+    <t>Josh anticipates KFC’s next big move - KFC Waffle House Hash Brown Double Down! FFF #004 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Tell KFC that you want to make the Hash Brown Double Down happen! https://ctt.ac/R42OT Watch today's GMMORE: Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>KFC Waffle House Hash Brown Double Down Taste Test | FUTURE FAST FOOD</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eQxQoYKpoag</t>
+  </si>
+  <si>
+    <t>Thanks to the National Pork Board for sponsoring today’s episode! Incorporate pork into your healthy diet. Visit https://www.pork.org/cooking/ to learn more. The question to ask this summer is: Will It BBQ? GMM #1550 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/w2t1AZyRpVk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Will It BBQ? Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ReJzgKpKxDU</t>
+  </si>
+  <si>
+    <t>We’re putting hot summer products to the test to find the 1 star vs. 5 star items! GMM #1551 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/OXOr0HkOeEs Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>1 Star vs. 5 Star Summer Products Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8q8hEuTxLmg</t>
+  </si>
+  <si>
+    <t>Can we match the celebrity to their favorite snacks with just a taste test? GMM #1552 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/1UWO2-z9RVM Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Celebrity Favorite Snacks Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=80_6idHuaXE</t>
+  </si>
+  <si>
+    <t>We’re settling the debate once and for all with a Texas Roadhouse vs. Outback Steakhouse Taste Test. Find out who will be the Food Feuds champ! GMM #1553 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/_4m6nLWulL4 Click the bell icon so you'll know when we add a new episode! Get The Look! Roadhouse Ronda: * Shirt: https://amzn.to/2XEZYDO * Hat: https://amzn.to/2XAdtV5 Outback Beck: * Shirt: https://amzn.to/2Fxyc1E * Shorts: https://amzn.to/2x9sjmL Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Texas Roadhouse vs. Outback Steakhouse Taste Test | FOOD FEUDS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xaG0hRYaeIE</t>
+  </si>
+  <si>
+    <t>Where in the world does Pizza Hut put Doritos on their pies? It’s an International Taste Test time! GMM #1554 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/1mKZQNlAX8A Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>International Pizza Hut Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Ka-f7PhLMwo</t>
+  </si>
+  <si>
+    <t>Will Ellie or Christine win the Brandless.com vs. Name Brand Game? GMM #1555 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/kILRsYGZByk Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Brandless.com vs. Name Brand Products (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rvtT_aagW_U</t>
+  </si>
+  <si>
+    <t>We’re putting our buds to the test to determine what’s the best cheese for your burger! GMM #1556 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/cMB4AqCPfCs Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What's The Best Cheese For Your Burger? (TEST)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wgOhw4OABeE</t>
+  </si>
+  <si>
+    <t>The Supreme Food Court is in session with The Try Guys! GMM #1557 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out The Try Guys’ new book, The Hidden Power of F*cking Up, available now. And follow The Try Guys on social media! Twitter: @tryguys Instagram: @tryguys Check out The Try Guys on tour! https://tryguys.com/pages/tour Subscribe to The Try Guys! https://www.youtube.com/channel/UCpi8TJfiA4lKGkaXs__YdBA?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/2kZL3WvhDek Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Supreme Food Court ft. The Try Guys</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AqjpEmHHvgA</t>
+  </si>
+  <si>
+    <t>Can Will and Steve guess the mystery sunscreen in this challenge? GMM #1558 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Subscribe to The Valleyfolk! https://www.youtube.com/channel/UCkEXXbo1QOTesV8h2hkN-1g?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/WPScYrrO5tA Click the bell icon so you'll know when we add a new episode! Get the Product! * Tickle Me Elmo: https://amzn.to/2Ybnlln Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>Mystery Sunscreen Challenge</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gsJ-JjQQWF0</t>
+  </si>
+  <si>
+    <t>The shuffleboard is back! Can we slip &amp; slide our way to guessing when these swimsuits from the last 100 years were popular? GMM #1559 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/s7fJyhyvQsA Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>100 Years of Swimsuits (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5qmyXYRzxQw</t>
+  </si>
+  <si>
+    <t>Our ultimate BBQ sauce taste test will get you through summer at the grill! GMM #1560 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/m79cHJrtc58 Click the bell icon so you'll know when we add a new episode! Get the Products! * Sweet Baby Ray’s Original Flavor: https://amzn.to/2FJYb6f * Kraft Original Flavor: https://amzn.to/2Ngn3Zk * KC Masterpiece Original Flavor: https://amzn.to/2FuvolO * Jack Daniels Original No. 7 Original Flavor: https://amzn.to/2JcuEmi * Stubbs Original Flavor: https://amzn.to/2NcQj3d * Head Country Original Flavor: https://amzn.to/2XsLtTr * Famous Dave’s Original Flavor: https://amzn.to/2X54rQt * Bulls-Eye Original Flavor: https://amzn.to/2XwFrB8 Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</t>
+  </si>
+  <si>
+    <t>What's The Best BBQ Sauce? Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=n6m8LytZM3o</t>
+  </si>
+  <si>
+    <t>Smosh's very own Courtney and Shayne are about to stretch these things to their limit to see when they'll break. GMM #1561 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Shayne &amp; Courtney on Smosh! https://www.youtube.com/user/smosh And follow them on social media Twitter: @Co_Mill &amp; @supershayne Instagram: @Co_Mill &amp; @shaynetopp See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/DdjTrow_f9o Click the bell icon so you'll know when we add a new episode! Get the Products! * Stretch Armstrong: https://amzn.to/2X7k4qw * Slinky Jr.: https://amzn.to/2YdMEDa * Pantyhose: https://amzn.to/2XbzxG0 * Bubble Tape: https://amzn.to/2NuqKLh * Stretch DVD: https://amzn.to/2FAzQzx Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>How Far Will It Stretch? (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wNzXsEQQE-o</t>
+  </si>
+  <si>
+    <t>Will a Chipotle funnel cake pass our taste test? GMM #1562 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/jj_cUGvfn1k Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Will It Funnel Cake? Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PWuDXPAc7vg</t>
+  </si>
+  <si>
+    <t>Shando joins us for a hilarious game of fill in the blank with kids’ summer camp letters! GMM #1563 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/mdT-iaKOZ84 Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Hilarious Kids' Summer Camp Letters (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ahw2nRNHZVY</t>
+  </si>
+  <si>
+    <t>Which cold brew coffee tops the taste test charts?! GMM #1564 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/oWkMeVKsg2U Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Cold Brew Coffee Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=HH_CJlX85Ho</t>
+  </si>
+  <si>
+    <t>What happens to pickle juice when it goes through a water filter? GMM #1565 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/UTP97NNviEQ Click the bell icon so you'll know when we add a new episode! Get the products! * Water Pitchers: https://amzn.to/2X5vOKa * Water Filters: https://amzn.to/2YdMNGI * Coyote Urine: https://amzn.to/2IPlgGs Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Putting Weird Things Through A Water Filter #3 (TEST)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pP_ZaC7aK20</t>
+  </si>
+  <si>
+    <t>We challenge Dylan Sprouse to spot the identical twin! GMM #1566 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Dylan in ‘Turandot,’ in theaters soon! And follow him on social media! Twitter: @dylansprouse Instagram: @dylansprouse See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/zFEo8OSI7SA Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Can We Spot The Identical Twin? (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cvEFLYEUL2o</t>
+  </si>
+  <si>
+    <t>Matt and Emily are ready for the summer blockbuster movie challenge… are you? GMM #1567 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/b3415im9RNM Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Summer Blockbuster Movie Challenge</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sFIVaycU4I8</t>
+  </si>
+  <si>
+    <t>Ice Cream Trucks have so many delicious options so obviously we need to do a taste test to determine the best one! GMM #1568 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/t5QubO-fHGg Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Ice Cream Truck Taste Test: Round 1</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=h-vFb43txo8</t>
+  </si>
+  <si>
+    <t>Which classic ice cream truck treat will win the Gold Cone?! GMM #1569 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Link turning into a human-sized ice cream sundae! http://bit.ly/RL_HumanSundae See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/ZSNf8NiXaSk Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Ice Cream Truck Taste Test: Finals</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=16fG_KIPa2c</t>
+  </si>
+  <si>
+    <t>Can Mythical Chef Josh and Smosh’s Shayne Topp guess the Scoville ranking of these hot sauces? GMM #1570 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Josh in Future Fast Food! https://www.youtube.com/watch?v=38DRQWl8n6Q&amp;list=PLJ49NV73ttrv4d8KDalwVvOIFg__FgJt5&amp;index=2&amp;t=0s And check out Shayne on Smosh! https://www.youtube.com/user/smosh And follow them both on social media! @mythicalchefjosh @shaynetopp See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/_U2nbcAmgOo Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Can We Guess the Heat of Hot Peppers? (CHALLENGE)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=soePexjeRgM</t>
+  </si>
+  <si>
+    <t>Which swim goggles can withstand our shark bite test?! GMM #1571 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Get the Damnyell &amp; Richard Tee! https://www.amazon.com/MYTHICAL-Damnyell-Richard-Tee/dp/B07DVYW47G Watch today's GMMORE: https://youtu.be/L6w6_ufnnuc Click the bell icon so you'll know when we add a new episode! Get the Products! * Speedo Vanquisher 2.0 Swim Goggle: https://amzn.to/2YbJZdm * Aegend Swim Goggles: https://amzn.to/2J9Vs6L * Michael Phelps Xceed Goggles: https://amzn.to/2XaDZFg * The Friendly Swede Goggles: https://amzn.to/2IRlm0l * TYR Transition Lens Goggles: https://amzn.to/2xequom Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Which Swim Goggles Are The Best? (TEST)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=15lNHHuihKc</t>
+  </si>
+  <si>
+    <t>Is it a hairless cat or a baby?... Can Gigi Gorgeous figure out What’s In My Suitcase?! GMM #1572 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Gigi’s new book ‘He Said, She Said: Lessons, Stories, and Mistakes from My Transgender Journey,’ available now! And visit Gigi’s YouTube Channel! https://www.youtube.com/gigigorgeous And follow her on social media! Twitter: @TheGigiGorgeous Instagram: @gigigorgeous Facebook: @GigiGorgeous See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/oT4z-TRsKmo Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>What's In My Suitcase? (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Uo0Ur7bSjII</t>
+  </si>
+  <si>
+    <t>Stevie and Smosh’s Courtney Miller taste test frozen fruit popsicles! GMM #1573 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Courtney on Smosh! https://www.youtube.com/user/smosh Join the Mythical Society: https://www.mythicalsociety.com/ And follow Stevie and Courtney on social media! @StevieWLevine @Co_Mill See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Frozen Fruit Popsicles Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5tD6Yttuy9Y</t>
+  </si>
+  <si>
+    <t>Can you guess what happens to a raw egg when you leave it in a hot car for a month? GMM #1574 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ http://www.bleakcreek.com Watch today's GMMORE: https://youtu.be/whm7uD29fBc Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Leaving Things In A Hot Car For A Month</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vR8owIdd6jo</t>
+  </si>
+  <si>
+    <t>What happens when we switch up the classic wet and dry foods? GMM #1575 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ http://www.bleakcreek.com Watch today's GMMORE: https://youtu.be/WvSfLltC7sU Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Wet Dry Food vs. Dry Wet Food Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=oU7ZHbtJ0Ho</t>
+  </si>
+  <si>
+    <t>Who will conquer the nasty balloon dart challenge? GMM #1576 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/a9DRj1hnxSU See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Nasty Balloon Dart Challenge</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aCEpiVC1VnU</t>
+  </si>
+  <si>
+    <t>Who will win the weirdest fair food taste test? GMM #1577 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/viqwiNzEXHg Click the bell icon so you'll know when we add a new episode! Get a copy of our new novel, The Lost Causes of Bleak Creek @ http://www.bleakcreek.com See Rhett &amp; Link play live in your city: tour tickets @ https://mythical.com/pages/tour Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Rhett &amp; Link: Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Weirdest Fair Foods Taste Test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3yy6jEo_ylc</t>
+  </si>
+  <si>
+    <t>Macaulay Culkin joins Rhett and Link to see who can win the bunny roulette challenge. GMM #1578 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Macaulay Culkin's official lifestyle website: https://bunnyears.com/ And follow Macaulay Culkin on social media! Twitter: @IncredibleCulk Instagram: @culkamania Facebook: @bunnyearsdotcom YouTube: https://www.youtube.com/channel/UCsCw3J3T3XFLgKm2te7TrTQ Watch today's GMMORE: https://youtu.be/7w-kIGSa4ac Click the bell icon so you'll know when we add a new episode! See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Can We Bet On What This Bunny Wants? (GAME)</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nurBtIDbeVk</t>
+  </si>
+  <si>
+    <t>Who will get dunked in the dirty water during this fill in the blank tank challenge? GMM #1579 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/Efc7T5BK1Do Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</t>
+  </si>
+  <si>
+    <t>Dirty Water Dunk Tank Challenge</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1yTDzs4BtCc</t>
+  </si>
+  <si>
+    <t>GMMoreLink</t>
+  </si>
+  <si>
+    <t>GMMLink</t>
+  </si>
+  <si>
+    <t>TextJoin</t>
   </si>
 </sst>
 </file>
@@ -4927,8 +5525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8774,10 +9372,1699 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46369AA0-EE19-6646-B29C-D1094DEF9E8C}">
+  <dimension ref="A1:N67"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>1476</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1477</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>1478</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>43684.514432870368</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="M3" t="str">
+        <f>RIGHT(E3,LEN(E3)-FIND("GMM #",E3)-4)</f>
+        <v>1579 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/Efc7T5BK1Do Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N3" t="str">
+        <f>LEFT(M3,4)</f>
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>43683.448946759258</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1472</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>1471</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1470</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M66" si="0">RIGHT(E4,LEN(E4)-FIND("GMM #",E4)-4)</f>
+        <v>1578 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Macaulay Culkin's official lifestyle website: https://bunnyears.com/ And follow Macaulay Culkin on social media! Twitter: @IncredibleCulk Instagram: @culkamania Facebook: @bunnyearsdotcom YouTube: https://www.youtube.com/channel/UCsCw3J3T3XFLgKm2te7TrTQ Watch today's GMMORE: https://youtu.be/7w-kIGSa4ac Click the bell icon so you'll know when we add a new episode! See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N66" si="1">LEFT(M4,4)</f>
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>43681.51326388889</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1468</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>1577 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/viqwiNzEXHg Click the bell icon so you'll know when we add a new episode! Get a copy of our new novel, The Lost Causes of Bleak Creek @ http://www.bleakcreek.com See Rhett &amp; Link play live in your city: tour tickets @ https://mythical.com/pages/tour Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical Merch at https://mythical.com and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Rhett &amp; Link: Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>43677.581550925926</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>1464</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>1576 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/a9DRj1hnxSU See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43676.630266203705</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>1461</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>1575 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ http://www.bleakcreek.com Watch today's GMMORE: https://youtu.be/WvSfLltC7sU Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>43672.604178240741</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1460</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1459</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>1458</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>1574 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ http://www.bleakcreek.com Watch today's GMMORE: https://youtu.be/whm7uD29fBc Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>43671.461944444447</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>1456</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1455</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>1573 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Courtney on Smosh! https://www.youtube.com/user/smosh Join the Mythical Society: https://www.mythicalsociety.com/ And follow Stevie and Courtney on social media! @StevieWLevine @Co_Mill See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>43669.455150462964</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1453</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1452</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>1572 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Gigi’s new book ‘He Said, She Said: Lessons, Stories, and Mistakes from My Transgender Journey,’ available now! And visit Gigi’s YouTube Channel! https://www.youtube.com/gigigorgeous And follow her on social media! Twitter: @TheGigiGorgeous Instagram: @gigigorgeous Facebook: @GigiGorgeous See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/oT4z-TRsKmo Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>43665.566782407404</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>1450</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>1571 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Get the Damnyell &amp; Richard Tee! https://www.amazon.com/MYTHICAL-Damnyell-Richard-Tee/dp/B07DVYW47G Watch today's GMMORE: https://youtu.be/L6w6_ufnnuc Click the bell icon so you'll know when we add a new episode! Get the Products! * Speedo Vanquisher 2.0 Swim Goggle: https://amzn.to/2YbJZdm * Aegend Swim Goggles: https://amzn.to/2J9Vs6L * Michael Phelps Xceed Goggles: https://amzn.to/2XaDZFg * The Friendly Swede Goggles: https://amzn.to/2IRlm0l * TYR Transition Lens Goggles: https://amzn.to/2xequom Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>43664.584918981483</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>1447</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>1446</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>1570 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Josh in Future Fast Food! https://www.youtube.com/watch?v=38DRQWl8n6Q&amp;list=PLJ49NV73ttrv4d8KDalwVvOIFg__FgJt5&amp;index=2&amp;t=0s And check out Shayne on Smosh! https://www.youtube.com/user/smosh And follow them both on social media! @mythicalchefjosh @shaynetopp See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/_U2nbcAmgOo Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="1"/>
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>43662.513275462959</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>1444</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>1569 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Link turning into a human-sized ice cream sundae! http://bit.ly/RL_HumanSundae See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/ZSNf8NiXaSk Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="1"/>
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>43658.778703703705</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1441</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>1440</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>1568 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/t5QubO-fHGg Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="1"/>
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>43656.687465277777</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>1438</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>1567 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/b3415im9RNM Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="1"/>
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>43655.497118055559</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>1435</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>1434</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>1566 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Dylan in ‘Turandot,’ in theaters soon! And follow him on social media! Twitter: @dylansprouse Instagram: @dylansprouse See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/zFEo8OSI7SA Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="1"/>
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>43651.444618055553</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>1565 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/UTP97NNviEQ Click the bell icon so you'll know when we add a new episode! Get the products! * Water Pitchers: https://amzn.to/2X5vOKa * Water Filters: https://amzn.to/2YdMNGI * Coyote Urine: https://amzn.to/2IPlgGs Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="1"/>
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>43649.615590277775</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>1429</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>1564 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/oWkMeVKsg2U Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="1"/>
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>43648.439212962963</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>1563 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/mdT-iaKOZ84 Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="1"/>
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>43644.632187499999</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1423</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>1422</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="0"/>
+        <v>1562 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/jj_cUGvfn1k Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="1"/>
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>43643.471782407411</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="0"/>
+        <v>1561 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out Shayne &amp; Courtney on Smosh! https://www.youtube.com/user/smosh And follow them on social media Twitter: @Co_Mill &amp; @supershayne Instagram: @Co_Mill &amp; @shaynetopp See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/DdjTrow_f9o Click the bell icon so you'll know when we add a new episode! Get the Products! * Stretch Armstrong: https://amzn.to/2X7k4qw * Slinky Jr.: https://amzn.to/2YdMEDa * Pantyhose: https://amzn.to/2XbzxG0 * Bubble Tape: https://amzn.to/2NuqKLh * Stretch DVD: https://amzn.to/2FAzQzx Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/ Get the GMM Set Gear! * Apple AirPort Extreme: https://amzn.to/2NnIvvk * Apple iPad Pro (12.9-inch, Wi-Fi, 64GB) - Space Gray (Latest Model) - MTEL2LL/A: https://amzn.to/2NnKXlw * Guardian Industrial Products DH-CP-4 3 Channel Rubber Cable Ramp (Straight): https://amzn.to/2NdshoR * Cartoni Focus HD Fluid Head with 3 Tube Ultra-Light Tripod, Mid-Level Spreader and Soft Case - Black: https://amzn.to/2X4i7X8 * ARRI SkyPanel S60-C LED Softlight (Blue/Silver, Edison): https://amzn.to/2YgM3km * Chef-Master 90050 Professional Heat Lamp, Silver: https://amzn.to/2Xa1Wwr * Samsung UN40H5003 40-Inch 1080p LED TV (2014 Model): https://amzn.to/2NdMU4e * Sony LMDA170 17" Production Video LCD Monitor, 16:9 Native Aspect Ratio, 1080p Resolution: https://amzn.to/2YlB9tH * Behringer Xenyx 1002 Premium 10-Input 2-Bus Mixer with XENYX Mic Preamps and British Eqs: https://amzn.to/2Yeeqzl * Elgato Game Capture Card HD60 S - Stream and Record in 1080p60, for PlayStation 4, Xbox One &amp; Xbox 360 (Renewed): https://amzn.to/2NdOBP6 * Pyle Universal Speaker Stand Mount Holder - Heavy Duty Tripod w/ Adjustable Height from 40” to 71” and 35mm Compatible Insert - Easy Mobility Safety PIN and Knob Tension Locking for Stability PSTND2: https://amzn.to/2JcCpce * JBL EON612 Portable 12" 2-Way Multipurpose Self-Powered Sound Reinforcement: https://amzn.to/2Ndluvm * Bolt 500 XT 3G-SDI/HDMI Wireless TX/RX: https://amzn.to/2J1OeSk * Voigtlaender 17,5/0,95 Nokton 17.5 mm-17.5 mm Lens: https://amzn.to/2JjUCEP * Blackmagic Design Micro Converter SDI to HDMI (with Power Supply) BMD-CONVCMIC/SH/WPSU: https://amzn.to/2J6iw6y * Panasonic H-HSA35100 F2.8 II ASPH 35-100mm Mirrorless Micro Four Thirds Mount POWER Optical I.S. LUMIX G X VARIO Professional Lens: https://amzn.to/2RAhIul * PANASONIC LUMIX Professional 12-35mm Camera Lens G X VARIO II, F2.8 ASPH, Dual I.S. 2.0 with Power O.I.S., Mirrorless Micro Four Thirds, H-HSA12035 (2017 Model, Black): https://amzn.to/2J9WH5S * Decimator Design DMON-12S | 12 Channel Multi Viewer with HDMI SDI Outputs: https://amzn.to/2J9Xkwg * Decimator MD-HX HDMI and SDI Cross Converter with Scaling &amp; Frame Rate Conversion: https://amzn.to/2Ymj52c * PANASONIC LUMIX GH4 Body 4K Mirrorless Camera, 16 Megapixels, 3 Inch Touch LCD, DMC-GH4KBODY (USA Black): https://amzn.to/2WZjlD6 * Blue Microphones Mouse Microphone Kc: https://amzn.to/2Ybu12I</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="1"/>
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>43641.56417824074</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>1416</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="0"/>
+        <v>1560 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/m79cHJrtc58 Click the bell icon so you'll know when we add a new episode! Get the Products! * Sweet Baby Ray’s Original Flavor: https://amzn.to/2FJYb6f * Kraft Original Flavor: https://amzn.to/2Ngn3Zk * KC Masterpiece Original Flavor: https://amzn.to/2FuvolO * Jack Daniels Original No. 7 Original Flavor: https://amzn.to/2JcuEmi * Stubbs Original Flavor: https://amzn.to/2NcQj3d * Head Country Original Flavor: https://amzn.to/2XsLtTr * Famous Dave’s Original Flavor: https://amzn.to/2X54rQt * Bulls-Eye Original Flavor: https://amzn.to/2XwFrB8 Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="1"/>
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>43637.664085648146</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>1413</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="0"/>
+        <v>1559 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Watch today's GMMORE: https://youtu.be/s7fJyhyvQsA Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="1"/>
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>43637.125208333331</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>1410</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="0"/>
+        <v>1558 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Subscribe to The Valleyfolk! https://www.youtube.com/channel/UCkEXXbo1QOTesV8h2hkN-1g?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/WPScYrrO5tA Click the bell icon so you'll know when we add a new episode! Get the Product! * Tickle Me Elmo: https://amzn.to/2Ybnlln Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="1"/>
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>43634.709687499999</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="0"/>
+        <v>1557 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 Check out The Try Guys’ new book, The Hidden Power of F*cking Up, available now. And follow The Try Guys on social media! Twitter: @tryguys Instagram: @tryguys Check out The Try Guys on tour! https://tryguys.com/pages/tour Subscribe to The Try Guys! https://www.youtube.com/channel/UCpi8TJfiA4lKGkaXs__YdBA?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/2kZL3WvhDek Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="1"/>
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>43630.573506944442</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1406</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>1404</v>
+      </c>
+      <c r="M26" t="str">
+        <f t="shared" si="0"/>
+        <v>1556 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/cMB4AqCPfCs Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="1"/>
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>43629.51898148148</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="M27" t="str">
+        <f t="shared" si="0"/>
+        <v>1555 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/kILRsYGZByk Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="1"/>
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>43627.489594907405</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>1398</v>
+      </c>
+      <c r="M28" t="str">
+        <f t="shared" si="0"/>
+        <v>1554 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/1mKZQNlAX8A Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="1"/>
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>43623.553576388891</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="M29" t="str">
+        <f t="shared" si="0"/>
+        <v>1553 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/_4m6nLWulL4 Click the bell icon so you'll know when we add a new episode! Get The Look! Roadhouse Ronda: * Shirt: https://amzn.to/2XEZYDO * Hat: https://amzn.to/2XAdtV5 Outback Beck: * Shirt: https://amzn.to/2Fxyc1E * Shorts: https://amzn.to/2x9sjmL Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="1"/>
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>43622.456354166665</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="0"/>
+        <v>1552 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/1UWO2-z9RVM Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="1"/>
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>43620.514166666668</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>1390</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>1389</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="0"/>
+        <v>1551 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/OXOr0HkOeEs Click the bell icon so you'll know when we add a new episode! Want more GMM? Check out these playlists: Season 15 - https://www.youtube.com/playlist?list=PLJ49NV73ttrvfAOYCnPCjbWuoldJvinRj Will It? - https://www.youtube.com/playlist?list=PLJ49NV73ttrucP6jJ1gjSqHmhlmvkdZuf Taste Tests! - https://www.youtube.com/playlist?list=PLJ49NV73ttrsUefw67wH_pnEJ5KwJZ7lN Fancy Fast Food - https://www.youtube.com/playlist?list=PLJ49NV73ttrvsfEo9x6FR7HURKOHQRnHO Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="1"/>
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>43616.477638888886</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>1386</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="0"/>
+        <v>1550 Subscribe to GMM: https://www.youtube.com/user/rhettandlink2?sub_confirmation=1 See Rhett &amp; Link play live in your city: tour tickets @ https://www.rhettandlinklive.com/ Watch today's GMMORE: https://youtu.be/w2t1AZyRpVk Click the bell icon so you'll know when we add a new episode! Want more GMM? Watch this season from the start: http://bit.ly/GMM_Season15 Pick up official GMM and Mythical merch at https://mythical.store and https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Join the Mythical Society: https://www.mythicalsociety.com/ Follow Mythical:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Dana Schechter https://www.danaschechter.com/ Intro &amp; Outro Music by Mark Byers http://www.markaholic.com/ Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="1"/>
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>43680.125081018516</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="M33" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N33" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>43684.635879629626</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>1380</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="0"/>
+        <v>1357 Watch today's GMMore: https://youtu.be/NaQViFWuO9g Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="1"/>
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>43687.125231481485</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="M35" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N35" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>43741.60087962963</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>1374</v>
+      </c>
+      <c r="M36" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N36" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>43741.601655092592</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="M37" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N37" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>43754.490486111114</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="M38" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N38" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>43754.490578703706</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="M39" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N39" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>43754.490983796299</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>1361</v>
+      </c>
+      <c r="M40" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N40" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>43833.438356481478</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="0"/>
+        <v>1358 Watch today's GMMore: https://youtu.be/qHTPTwiElU4 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="1"/>
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>43833.438379629632</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>1356</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>1355</v>
+      </c>
+      <c r="M42" t="str">
+        <f t="shared" si="0"/>
+        <v>1355 Watch today's GMMore: https://youtu.be/nMpGrm_2BQM Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="1"/>
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>43833.438425925924</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="M43" t="str">
+        <f t="shared" si="0"/>
+        <v>1352 Watch today's GMMore: https://youtu.be/2gVLBIwYXfY Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="1"/>
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>43833.438437500001</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="M44" t="str">
+        <f t="shared" si="0"/>
+        <v>1359 Thanks to Threadbanger for hosting GMM today! Check them out: https://www.youtube.com/ThreadBanger https://twitter.com/Threadbanger Watch today's GMMore: https://youtu.be/x2rcnIHjTTA Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="1"/>
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>43833.438483796293</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="M45" t="str">
+        <f t="shared" si="0"/>
+        <v>1354 Watch today's GMMore: https://youtu.be/nZ0n5PelEqc Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="1"/>
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>43833.438518518517</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>1343</v>
+      </c>
+      <c r="M46" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N46" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>43833.438530092593</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="M47" t="str">
+        <f t="shared" si="0"/>
+        <v>1346 Watch today's GMMore: https://youtu.be/hcJIGQzH4SQ Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="1"/>
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>43833.43854166667</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>1338</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="M48" t="str">
+        <f t="shared" si="0"/>
+        <v>1351 Watch today's GMMore: https://youtu.be/x81k9pKkkWQ Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="1"/>
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>43833.43854166667</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="M49" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N49" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>43833.438564814816</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="M50" t="str">
+        <f t="shared" si="0"/>
+        <v>1349 Watch today's GMMore: https://youtu.be/1EvYN7E18AI Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="1"/>
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>43833.438564814816</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>1328</v>
+      </c>
+      <c r="M51" t="str">
+        <f t="shared" si="0"/>
+        <v>1350 Thanks to Sean Evans for hosting GMS today! Check him out at: Hot Ones: https://goo.gl/xjU8rR Twitter: https://twitter.com/seanseaevans Watch today's GMMore: https://youtu.be/a74US2GPxs4 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="1"/>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>43833.438599537039</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>1325</v>
+      </c>
+      <c r="M52" t="str">
+        <f t="shared" si="0"/>
+        <v>1347 Thanks to the Try Guys for hosting GMM today! Check out their new channel today: https://goo.gl/pdUjr4 Watch today's GMMore: https://youtu.be/9Nn4F5F6klg Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="1"/>
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>1322</v>
+      </c>
+      <c r="M53" t="str">
+        <f t="shared" si="0"/>
+        <v>1344 Thanks to Jon &amp; Noah for hosting today's GMS, check them out at: Noah Cyrus: https://www.instagram.com/noahcyrus/ https://twitter.com/noahcyrus/ https://facebook.com/noahcyrus/ Jon Cozart: https://www.youtube.com/user/Paint Watch today's GMMore: https://youtu.be/mLvbZAdGsZY Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Check our Noah's latest single, Team, here: Spotify: http://smarturl.it/AlwaysBeOnYourTeam/spotify Apple Music: http://smarturl.it/AlwaysBeOnYourTeam/applemusic iTunes: http://smarturl.it/AlwaysBeOnYourTeam/itunes Amazon: http://smarturl.it/AlwaysBeOnYourTeam/az Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="1"/>
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>1319</v>
+      </c>
+      <c r="M54" t="str">
+        <f t="shared" si="0"/>
+        <v>1353 Thanks to De'arra &amp; Ken for hosting today's episode! Check them out: De'arra &amp; Ken 4 Life: https://goo.gl/Wsta5j DK4L Vlogs: https://goo.gl/G8V9LR Watch today's GMMore: https://youtu.be/ELBP8yU-RI4 Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="1"/>
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>1316</v>
+      </c>
+      <c r="M55" t="str">
+        <f t="shared" si="0"/>
+        <v>1345 Watch today's GMMore: https://youtu.be/Uzq7F3ImZRA Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" si="1"/>
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>1313</v>
+      </c>
+      <c r="M56" t="str">
+        <f t="shared" si="0"/>
+        <v>1340 Watch today's GMMore: https://youtu.be/679xaKECVHo Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="1"/>
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>1310</v>
+      </c>
+      <c r="M57" t="str">
+        <f t="shared" si="0"/>
+        <v>1341 Thanks to Safiya &amp; Tyler for hosting GMS! Check them out at: Safiya's Channel: https://www.youtube.com/safiyanygaard Tyler's Channel: https://www.youtube.com/channel/UCc6BTuuTzfMLKj_RgwuDnQw Watch today's GMMore: https://youtu.be/OXGDwVKHAEU Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" si="1"/>
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>1307</v>
+      </c>
+      <c r="M58" t="str">
+        <f t="shared" si="0"/>
+        <v>1342 Watch today's GMMore: https://youtu.be/O5Xia4_tqzY Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N58" t="str">
+        <f t="shared" si="1"/>
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="M59" t="str">
+        <f t="shared" si="0"/>
+        <v>1338 Thanks to Nick and Kiersey for hosting this episode of Good Mythical Summer! Check out their movie "Hearts Beat Loud" in theaters now. Watch the trailer here: https://www.youtube.com/watch?v=PXNOg_SK7Vs Watch today's GMMore: https://youtu.be/1yAJ4MH8mss Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N59" t="str">
+        <f t="shared" si="1"/>
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>1301</v>
+      </c>
+      <c r="M60" t="str">
+        <f t="shared" si="0"/>
+        <v>1343 Watch today's GMMore: https://youtu.be/FNlwbta04Po Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="1"/>
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="M61" t="str">
+        <f t="shared" si="0"/>
+        <v>1333 Get our limited edition Summer Camp tee at http://mythical.store Watch today's GMMore: https://youtu.be/-humHGoKXzw Want more GMS? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="1"/>
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>1295</v>
+      </c>
+      <c r="M62" t="str">
+        <f t="shared" si="0"/>
+        <v>1337 Watch today's GMMore: https://youtu.be/QwNf7mWQmFM Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="1"/>
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="M63" t="str">
+        <f t="shared" si="0"/>
+        <v>1334 Watch today's GMMore: https://youtu.be/UXnc_HBjzPo Want more GMS? Watch from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" si="1"/>
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="M64" t="str">
+        <f t="shared" si="0"/>
+        <v>1348 Watch today's GMMore: https://youtu.be/976cBg_gwYM Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don't miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: 'The Mouse' by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N64" t="str">
+        <f t="shared" si="1"/>
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="M65" t="str">
+        <f t="shared" si="0"/>
+        <v>1336 Watch today's GMMore: https://youtu.be/o0P78KNN01M Want more GMS? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="1"/>
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M66" t="str">
+        <f t="shared" si="0"/>
+        <v>1335 Thanks to Lauren &amp; Alex for hosting this episode of Good Mythical Summer! Check them out here: LaurDIY: https://www.youtube.com/LaurDIY Alex Wassabi: https://www.youtube.com/wassabi Watch today's GMMore: https://youtu.be/KLSkvMzj0Ak Want more GMM? Watch this season from the start: http://bit.ly/GMS_2018 Pick up official GMM merch at https://mythical.store Get exclusive limited edition tees only at https://www.amazon.com/mythical Don’t miss our weekly podcast, Ear Biscuits: https://applepodcasts.com/earbiscuits Follow Rhett &amp; Link:  Instagram: https://instagram.com/mythical Facebook: https://facebook.com/mythical Twitter: https://twitter.com/mythical Tumblr: https://rhettandlink.tumblr.com Snapchat: @realrhettlink Website: https://mythical.com/ Check Out Our Other Mythical Channels: Good Mythical MORE: https://youtube.com/goodmythicalmore Rhett &amp; Link: https://youtube.com/rhettandlink Mythical: https://youtube.com/thisismythical Want to send us something? https://mythical.com/contact Submit your Wheel of Mythicality intro video here: http://bit.ly/GMMWheelIntroSUBMISSIONS Intro Animation by Digital Twigs: https://www.digitaltwigs.com Intro &amp; Outro Music by Jeff Zeigler &amp; Sarah Schimeneck https://www.jeffzeigler.com Supplemental Music from Extreme Production Music: https://www.extrememusic.com/ Mic: ‘The Mouse’ by Blue Microphones https://www.bluemic.com/mouse/</v>
+      </c>
+      <c r="N66" t="str">
+        <f t="shared" si="1"/>
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>43833.438622685186</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AA8892-3CBD-914A-97B0-ABA99B970016}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -12845,7 +15132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7D142B-1817-4B41-9B6B-B1ABD3656E7C}">
   <dimension ref="A1:M101"/>
   <sheetViews>
@@ -15217,7 +17504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K131"/>
   <sheetViews>

</xml_diff>